<commit_message>
:tada:[ADD] DFS/BFS - 음료수 얼려먹기
생각하는 방향은 맞았던거 같은데, 구현이 미숙하여 테스트케이스를 1개만 통과함.
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF3FDE-1C28-4A69-86DB-B09ED2110F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56317AD2-1F36-42E3-9B33-17B660BB388F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="1780" windowWidth="27660" windowHeight="15460" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -145,11 +145,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">
-정리한거 리뷰</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>github 관리</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -173,6 +168,14 @@
   </si>
   <si>
     <t>개념</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본을 리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS - 1개 (음료수 얼려 먹기)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1085,7 +1088,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:M10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1191,7 +1194,7 @@
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -1222,7 +1225,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="18"/>
       <c r="H4" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -1250,7 +1253,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>26</v>
@@ -1259,16 +1262,16 @@
         <v>26</v>
       </c>
       <c r="H5" s="47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="48"/>
       <c r="J5" s="49"/>
       <c r="K5" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
@@ -1410,7 +1413,7 @@
         <v>44419</v>
       </c>
       <c r="J9" s="45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" s="45"/>
       <c r="L9" s="45"/>
@@ -1432,27 +1435,35 @@
       <c r="B10" s="10">
         <v>3</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="10">
         <v>4</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="H10" s="11">
         <v>4</v>
       </c>
       <c r="I10" s="12">
-        <v>44420</v>
-      </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
+        <v>44423</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
       <c r="O10" s="12">
         <v>44420</v>
+      </c>
+      <c r="P10" s="12">
+        <v>44423</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>44421</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
:tada:[ADD] Sort - 위에서 아래로.
기본 정렬 라이브러리르 사용하여 쉽게 해결함.
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9D02F3-4866-4E55-9D5E-453271FDF78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6AC278-CA66-482E-B0E3-5A07B434565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -171,11 +171,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>원본을 리뷰</t>
+    <t>DFS - 1개 (음료수 얼려 먹기)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DFS - 1개 (음료수 얼려 먹기)</t>
+    <t>BFS - 1개 (미로 탈출)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본(책)을 리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정렬 - 개념, 1개 (위에서 아래로)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -632,7 +640,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -695,75 +703,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
@@ -1088,7 +1098,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1253,7 +1263,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>26</v>
@@ -1261,11 +1271,11 @@
       <c r="G5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="44" t="s">
         <v>31</v>
       </c>
@@ -1352,9 +1362,9 @@
       <c r="J7" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1379,12 +1389,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="51"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="35"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1412,12 +1422,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="53"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1447,12 +1457,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="51"/>
+      <c r="J10" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1473,13 +1483,21 @@
       <c r="B11" s="10">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>5</v>
       </c>
       <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="J11" s="34"/>
+      <c r="H11" s="11">
+        <v>5</v>
+      </c>
+      <c r="I11" s="12">
+        <v>44424</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="35"/>
@@ -1489,6 +1507,9 @@
       <c r="O11" s="12">
         <v>44424</v>
       </c>
+      <c r="P11" s="12">
+        <v>44424</v>
+      </c>
       <c r="Q11" s="12">
         <v>44424</v>
       </c>
@@ -1497,21 +1518,38 @@
       <c r="A12" s="2">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="10">
         <v>5</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>6</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="10">
         <v>3</v>
       </c>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="35"/>
+      <c r="H12" s="11">
+        <v>6</v>
+      </c>
+      <c r="I12" s="12">
+        <v>44425</v>
+      </c>
+      <c r="J12" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="57"/>
       <c r="N12" s="2">
         <v>6</v>
+      </c>
+      <c r="O12" s="12">
+        <v>44425</v>
+      </c>
+      <c r="P12" s="12">
+        <v>44425</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>44425</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.45">
@@ -1527,10 +1565,10 @@
       <c r="D13" s="2">
         <v>4</v>
       </c>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="35"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="56"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1551,10 +1589,10 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="35"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="56"/>
       <c r="N14" s="2">
         <v>8</v>
       </c>
@@ -1575,10 +1613,10 @@
       <c r="E15" s="2">
         <v>2</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="35"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="56"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -1599,10 +1637,10 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="35"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="56"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -1623,10 +1661,10 @@
       <c r="E17" s="2">
         <v>4</v>
       </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="56"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -1647,10 +1685,10 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="35"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="56"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -1673,10 +1711,10 @@
       <c r="E19" s="2">
         <v>6</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="35"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="56"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -1698,10 +1736,10 @@
       <c r="E20" s="2">
         <v>7</v>
       </c>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="35"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="56"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -1725,10 +1763,10 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="35"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="56"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -1756,10 +1794,10 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="35"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="56"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -1786,10 +1824,10 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="35"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="56"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -1815,10 +1853,10 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="35"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="56"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -1844,10 +1882,10 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="35"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="56"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -1872,10 +1910,10 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="35"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="56"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -1901,10 +1939,10 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="35"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="56"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -1930,10 +1968,10 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="35"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="56"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -1958,10 +1996,10 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="35"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="56"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -1988,10 +2026,10 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="35"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="56"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2018,10 +2056,10 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="35"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="56"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2048,10 +2086,10 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="35"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="56"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2078,10 +2116,10 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="35"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="56"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2108,10 +2146,10 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="35"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="56"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2138,10 +2176,10 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="35"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="56"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2168,10 +2206,10 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="35"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="56"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2198,10 +2236,10 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="35"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="56"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2224,10 +2262,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="35"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="56"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2249,10 +2287,10 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="35"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="56"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2271,10 +2309,10 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="35"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="56"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2294,10 +2332,10 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="34"/>
-      <c r="K41" s="34"/>
-      <c r="L41" s="34"/>
-      <c r="M41" s="35"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="56"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2318,10 +2356,10 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="35"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="56"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2342,10 +2380,10 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="35"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="56"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2362,10 +2400,10 @@
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="35"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="56"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2383,10 +2421,10 @@
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="34"/>
-      <c r="K45" s="34"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="35"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="56"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2404,10 +2442,10 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="35"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="56"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2424,10 +2462,10 @@
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="34"/>
-      <c r="K47" s="34"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="35"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="56"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -2444,10 +2482,10 @@
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="35"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="56"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -2464,10 +2502,10 @@
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="34"/>
-      <c r="K49" s="34"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="35"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="55"/>
+      <c r="M49" s="56"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -2485,10 +2523,10 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="35"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="55"/>
+      <c r="M50" s="56"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -2503,10 +2541,10 @@
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="35"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="56"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -2521,10 +2559,10 @@
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
-      <c r="M52" s="35"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="55"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="56"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -2539,10 +2577,10 @@
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="34"/>
-      <c r="K53" s="34"/>
-      <c r="L53" s="34"/>
-      <c r="M53" s="35"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="55"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="56"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -2557,10 +2595,10 @@
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="35"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="56"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -2575,10 +2613,10 @@
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="35"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="56"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -2593,10 +2631,10 @@
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="35"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="55"/>
+      <c r="L56" s="55"/>
+      <c r="M56" s="56"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -2611,10 +2649,10 @@
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="34"/>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="35"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="55"/>
+      <c r="M57" s="56"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -2629,10 +2667,10 @@
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="34"/>
-      <c r="M58" s="35"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="55"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="56"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -2647,10 +2685,10 @@
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="34"/>
-      <c r="K59" s="34"/>
-      <c r="L59" s="34"/>
-      <c r="M59" s="35"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="55"/>
+      <c r="L59" s="55"/>
+      <c r="M59" s="56"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -2665,10 +2703,10 @@
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-      <c r="M60" s="35"/>
+      <c r="J60" s="55"/>
+      <c r="K60" s="55"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="56"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -2681,10 +2719,10 @@
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="34"/>
-      <c r="M61" s="35"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="55"/>
+      <c r="L61" s="55"/>
+      <c r="M61" s="56"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -2700,10 +2738,10 @@
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="34"/>
-      <c r="K62" s="34"/>
-      <c r="L62" s="34"/>
-      <c r="M62" s="35"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="56"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -2718,10 +2756,10 @@
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="35"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="55"/>
+      <c r="L63" s="55"/>
+      <c r="M63" s="56"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -2736,10 +2774,10 @@
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="34"/>
-      <c r="K64" s="34"/>
-      <c r="L64" s="34"/>
-      <c r="M64" s="35"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="55"/>
+      <c r="L64" s="55"/>
+      <c r="M64" s="56"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -2753,10 +2791,10 @@
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="34"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="34"/>
-      <c r="M65" s="35"/>
+      <c r="J65" s="55"/>
+      <c r="K65" s="55"/>
+      <c r="L65" s="55"/>
+      <c r="M65" s="56"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -2765,10 +2803,10 @@
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="34"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
-      <c r="M66" s="35"/>
+      <c r="J66" s="55"/>
+      <c r="K66" s="55"/>
+      <c r="L66" s="55"/>
+      <c r="M66" s="56"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -2845,7 +2883,7 @@
       <c r="Q84" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="80">
     <mergeCell ref="J66:M66"/>
     <mergeCell ref="J60:M60"/>
     <mergeCell ref="J61:M61"/>
@@ -2890,7 +2928,6 @@
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="J34:M34"/>
     <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J12:M12"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="J14:M14"/>
     <mergeCell ref="J15:M15"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 8일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B721C25-E4A4-41BA-AA13-CECF0FBC877D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1D28A-52CC-4BD1-AE70-08D156289042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="7240" yWindow="4760" windowWidth="18210" windowHeight="15470" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -179,15 +179,24 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>원본(책)을 리뷰</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>정렬 - 개념, 1개 (위에서 아래로)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>정렬 - 2개 (성적 낮은 순서로 출력, 두 배열의 원소 교체)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이진 탐색 - 개념, 1개 (부품 찾기)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이진 탐색 - 떡볶이 떡 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 구현
+원본(책)을 리뷰</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1102,7 +1111,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:M13"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1267,7 +1276,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>26</v>
@@ -1538,7 +1547,7 @@
         <v>44425</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
@@ -1576,7 +1585,7 @@
         <v>44426</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -1598,24 +1607,44 @@
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="10">
         <v>8</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="10">
         <v>5</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="10">
         <v>1</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="30"/>
+      <c r="H14" s="11">
+        <v>8</v>
+      </c>
+      <c r="I14" s="12">
+        <v>44428</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="27"/>
       <c r="N14" s="2">
         <v>8</v>
+      </c>
+      <c r="O14" s="12">
+        <v>44429</v>
+      </c>
+      <c r="P14" s="12">
+        <v>44428</v>
+      </c>
+      <c r="Q14" s="12">
+        <v>44429</v>
+      </c>
+      <c r="R14" s="12">
+        <v>44429</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.45">
@@ -1625,7 +1654,7 @@
       <c r="B15" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="10">
         <v>9</v>
       </c>
       <c r="D15" s="2">
@@ -1634,10 +1663,18 @@
       <c r="E15" s="2">
         <v>2</v>
       </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30"/>
+      <c r="H15" s="11">
+        <v>9</v>
+      </c>
+      <c r="I15" s="12">
+        <v>44429</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="32"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -2904,7 +2941,7 @@
       <c r="Q84" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="79">
     <mergeCell ref="AB1:AJ1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
@@ -2933,7 +2970,6 @@
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="J23:M23"/>
     <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J14:M14"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="J16:M16"/>
     <mergeCell ref="J17:M17"/>
@@ -2988,6 +3024,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 9일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1D28A-52CC-4BD1-AE70-08D156289042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704F9056-F48C-4303-9350-B13CE5D0EEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="4760" windowWidth="18210" windowHeight="15470" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -697,95 +697,95 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1134,112 +1134,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58" t="s">
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58" t="s">
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52" t="s">
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="56" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:36" s="6" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="38"/>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="24" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="37"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="42"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1252,17 +1252,17 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="40"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="45"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A5" s="17"/>
@@ -1284,15 +1284,15 @@
       <c r="G5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="41" t="s">
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="42"/>
+      <c r="L5" s="47"/>
       <c r="M5" s="26" t="s">
         <v>32</v>
       </c>
@@ -1327,14 +1327,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="50"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1372,12 +1372,12 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="46" t="s">
+      <c r="J7" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1402,12 +1402,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="32"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1435,12 +1435,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="47" t="s">
+      <c r="J9" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="48"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="53"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1470,12 +1470,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="32"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1508,12 +1508,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="32"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1584,12 +1584,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="32"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1651,16 +1651,16 @@
       <c r="A15" s="2">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="10">
         <v>8</v>
       </c>
       <c r="C15" s="10">
         <v>9</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="10">
         <v>6</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="10">
         <v>2</v>
       </c>
       <c r="H15" s="11">
@@ -1669,14 +1669,26 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="32"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
       <c r="N15" s="2">
         <v>9</v>
+      </c>
+      <c r="O15" s="12">
+        <v>44430</v>
+      </c>
+      <c r="P15" s="12">
+        <v>44429</v>
+      </c>
+      <c r="Q15" s="12">
+        <v>44430</v>
+      </c>
+      <c r="R15" s="12">
+        <v>44430</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.45">
@@ -1695,10 +1707,10 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30"/>
+      <c r="J16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="58"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -1719,10 +1731,10 @@
       <c r="E17" s="2">
         <v>4</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="30"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="58"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -1743,10 +1755,10 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="30"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="58"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -1769,10 +1781,10 @@
       <c r="E19" s="2">
         <v>6</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="30"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="58"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -1794,10 +1806,10 @@
       <c r="E20" s="2">
         <v>7</v>
       </c>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="30"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="58"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -1821,10 +1833,10 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="30"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="58"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -1852,10 +1864,10 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="58"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -1882,10 +1894,10 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="30"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="58"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -1911,10 +1923,10 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="30"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="58"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -1940,10 +1952,10 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="30"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="58"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -1968,10 +1980,10 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="30"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="58"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -1997,10 +2009,10 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="30"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="58"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2026,10 +2038,10 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="30"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="58"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -2054,10 +2066,10 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="30"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -2084,10 +2096,10 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="30"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="58"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2114,10 +2126,10 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="30"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="58"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2144,10 +2156,10 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="30"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="58"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2174,10 +2186,10 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="30"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="58"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2204,10 +2216,10 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="29"/>
-      <c r="M34" s="30"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="58"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2234,10 +2246,10 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="30"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="58"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2264,10 +2276,10 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="30"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="58"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2294,10 +2306,10 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="30"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="58"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2320,10 +2332,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="30"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="58"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2345,10 +2357,10 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="29"/>
-      <c r="M39" s="30"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="58"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2367,10 +2379,10 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="30"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="58"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2390,10 +2402,10 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="30"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="58"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2414,10 +2426,10 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="30"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="58"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2438,10 +2450,10 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="30"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="58"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2458,10 +2470,10 @@
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="30"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="58"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2479,10 +2491,10 @@
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="30"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="58"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2500,10 +2512,10 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="30"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="58"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2520,10 +2532,10 @@
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="30"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="58"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -2540,10 +2552,10 @@
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="30"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="58"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -2560,10 +2572,10 @@
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="30"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="58"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -2581,10 +2593,10 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="30"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="58"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -2599,10 +2611,10 @@
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="30"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="58"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -2617,10 +2629,10 @@
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="30"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="58"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -2635,10 +2647,10 @@
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="30"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="57"/>
+      <c r="M53" s="58"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -2653,10 +2665,10 @@
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="30"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="57"/>
+      <c r="L54" s="57"/>
+      <c r="M54" s="58"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -2671,10 +2683,10 @@
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="30"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="57"/>
+      <c r="L55" s="57"/>
+      <c r="M55" s="58"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -2689,10 +2701,10 @@
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="29"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="30"/>
+      <c r="J56" s="57"/>
+      <c r="K56" s="57"/>
+      <c r="L56" s="57"/>
+      <c r="M56" s="58"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -2707,10 +2719,10 @@
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="30"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="57"/>
+      <c r="L57" s="57"/>
+      <c r="M57" s="58"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -2725,10 +2737,10 @@
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="30"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="57"/>
+      <c r="M58" s="58"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -2743,10 +2755,10 @@
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="30"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="58"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -2761,10 +2773,10 @@
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="30"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="57"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="58"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -2777,10 +2789,10 @@
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="30"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="58"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -2796,10 +2808,10 @@
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="29"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="30"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="58"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -2814,10 +2826,10 @@
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
-      <c r="L63" s="29"/>
-      <c r="M63" s="30"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="58"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -2832,10 +2844,10 @@
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="30"/>
+      <c r="J64" s="57"/>
+      <c r="K64" s="57"/>
+      <c r="L64" s="57"/>
+      <c r="M64" s="58"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -2849,10 +2861,10 @@
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="30"/>
+      <c r="J65" s="57"/>
+      <c r="K65" s="57"/>
+      <c r="L65" s="57"/>
+      <c r="M65" s="58"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -2861,10 +2873,10 @@
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
-      <c r="M66" s="30"/>
+      <c r="J66" s="57"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="57"/>
+      <c r="M66" s="58"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -2942,18 +2954,59 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
@@ -2968,59 +3021,18 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 10일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704F9056-F48C-4303-9350-B13CE5D0EEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA812858-CB93-4974-AF57-AA57A3814887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -197,6 +197,11 @@
   <si>
     <t>코드 구현
 원본(책)을 리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 구현
+obsidian에 리뷰</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,6 +701,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,74 +791,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1111,13 +1118,14 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="R16" activeCellId="1" sqref="Q16 R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.58203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.58203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.58203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.08203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.4140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.9140625" style="2" customWidth="1"/>
@@ -1134,112 +1142,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35" t="s">
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35" t="s">
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35" t="s">
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29" t="s">
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="32"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="54"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:36" s="6" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="32"/>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="24" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="42"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="36"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1247,53 +1255,53 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="45"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="39"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A5" s="17"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="46" t="s">
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="26" t="s">
+      <c r="L5" s="41"/>
+      <c r="M5" s="25" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="16"/>
@@ -1327,14 +1335,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="50"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="44"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1372,12 +1380,12 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="37"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1402,12 +1410,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1435,12 +1443,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="53"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="47"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1470,12 +1478,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="37"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1508,12 +1516,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1546,12 +1554,12 @@
       <c r="I12" s="12">
         <v>44425</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="26"/>
       <c r="N12" s="2">
         <v>6</v>
       </c>
@@ -1584,12 +1592,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1625,12 +1633,12 @@
       <c r="I14" s="12">
         <v>44428</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="26"/>
       <c r="N14" s="2">
         <v>8</v>
       </c>
@@ -1669,12 +1677,12 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -1695,24 +1703,36 @@
       <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>10</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="10">
         <v>7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="10">
         <v>3</v>
       </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="58"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
       <c r="N16" s="2">
         <v>10</v>
+      </c>
+      <c r="O16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="P16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="Q16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="R16" s="12">
+        <v>44431</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.45">
@@ -1731,10 +1751,10 @@
       <c r="E17" s="2">
         <v>4</v>
       </c>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="58"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -1755,10 +1775,10 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="58"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -1781,10 +1801,10 @@
       <c r="E19" s="2">
         <v>6</v>
       </c>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="58"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -1806,10 +1826,10 @@
       <c r="E20" s="2">
         <v>7</v>
       </c>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="58"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -1833,10 +1853,10 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="58"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -1864,10 +1884,10 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="58"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -1894,10 +1914,10 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="58"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="29"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -1923,10 +1943,10 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="58"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -1952,10 +1972,10 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="58"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="29"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -1980,10 +2000,10 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="58"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -2009,10 +2029,10 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="58"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2038,10 +2058,10 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="58"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -2066,10 +2086,10 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="58"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="29"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -2096,10 +2116,10 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="58"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2126,10 +2146,10 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="58"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="29"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2156,10 +2176,10 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="58"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="29"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2186,10 +2206,10 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="58"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="29"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2216,10 +2236,10 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="58"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="29"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2246,10 +2266,10 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="58"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="29"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2276,10 +2296,10 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="58"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="29"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2306,10 +2326,10 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="58"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="29"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2332,10 +2352,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="58"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="29"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2357,10 +2377,10 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="58"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="29"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2379,10 +2399,10 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="58"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="29"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2402,10 +2422,10 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="58"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="29"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2426,10 +2446,10 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="57"/>
-      <c r="K42" s="57"/>
-      <c r="L42" s="57"/>
-      <c r="M42" s="58"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="29"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2450,10 +2470,10 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="57"/>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="58"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="29"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2470,10 +2490,10 @@
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="58"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="29"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2491,10 +2511,10 @@
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="58"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="29"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2512,10 +2532,10 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="58"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="29"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2532,10 +2552,10 @@
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="58"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="29"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -2552,10 +2572,10 @@
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="57"/>
-      <c r="K48" s="57"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="58"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="29"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -2572,10 +2592,10 @@
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="57"/>
-      <c r="K49" s="57"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="58"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="29"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -2593,10 +2613,10 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="58"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="29"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -2611,10 +2631,10 @@
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="58"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="29"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -2629,10 +2649,10 @@
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="58"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="29"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -2647,10 +2667,10 @@
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="57"/>
-      <c r="K53" s="57"/>
-      <c r="L53" s="57"/>
-      <c r="M53" s="58"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="29"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -2665,10 +2685,10 @@
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="57"/>
-      <c r="M54" s="58"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="29"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -2683,10 +2703,10 @@
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="57"/>
-      <c r="K55" s="57"/>
-      <c r="L55" s="57"/>
-      <c r="M55" s="58"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="29"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -2701,10 +2721,10 @@
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="57"/>
-      <c r="K56" s="57"/>
-      <c r="L56" s="57"/>
-      <c r="M56" s="58"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="29"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -2719,10 +2739,10 @@
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="57"/>
-      <c r="M57" s="58"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="29"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -2737,10 +2757,10 @@
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-      <c r="M58" s="58"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="29"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -2755,10 +2775,10 @@
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="57"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="57"/>
-      <c r="M59" s="58"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="29"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -2773,10 +2793,10 @@
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="58"/>
+      <c r="J60" s="28"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="M60" s="29"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -2789,10 +2809,10 @@
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="57"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="57"/>
-      <c r="M61" s="58"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="29"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -2808,10 +2828,10 @@
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="58"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="29"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -2826,10 +2846,10 @@
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="58"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="28"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="29"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -2844,10 +2864,10 @@
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
-      <c r="L64" s="57"/>
-      <c r="M64" s="58"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="29"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -2861,10 +2881,10 @@
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="57"/>
-      <c r="K65" s="57"/>
-      <c r="L65" s="57"/>
-      <c r="M65" s="58"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="29"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -2873,10 +2893,10 @@
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="57"/>
-      <c r="K66" s="57"/>
-      <c r="L66" s="57"/>
-      <c r="M66" s="58"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="29"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -2954,59 +2974,18 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
@@ -3021,18 +3000,59 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 11일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704F9056-F48C-4303-9350-B13CE5D0EEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF017A-DF7A-42BF-9997-8259D567AEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="1880" yWindow="60" windowWidth="26830" windowHeight="19720" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -197,6 +197,15 @@
   <si>
     <t>코드 구현
 원본(책)을 리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 구현
+obsidian에 리뷰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다이나믹 프로그래밍 - 개념</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +690,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,6 +705,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1111,13 +1122,14 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.58203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.58203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.58203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.08203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.4140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.9140625" style="2" customWidth="1"/>
@@ -1216,11 +1228,11 @@
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="39"/>
       <c r="L3" s="39"/>
       <c r="M3" s="7"/>
@@ -1247,7 +1259,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="6"/>
@@ -1266,22 +1278,22 @@
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A5" s="17"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="54" t="s">
@@ -1293,7 +1305,7 @@
         <v>31</v>
       </c>
       <c r="L5" s="47"/>
-      <c r="M5" s="26" t="s">
+      <c r="M5" s="25" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="16"/>
@@ -1546,12 +1558,12 @@
       <c r="I12" s="12">
         <v>44425</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="26"/>
       <c r="N12" s="2">
         <v>6</v>
       </c>
@@ -1625,12 +1637,12 @@
       <c r="I14" s="12">
         <v>44428</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="26"/>
       <c r="N14" s="2">
         <v>8</v>
       </c>
@@ -1695,40 +1707,60 @@
       <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="10">
         <v>10</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="10">
         <v>7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="10">
         <v>3</v>
       </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="58"/>
+      <c r="H16" s="11">
+        <v>10</v>
+      </c>
+      <c r="I16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="J16" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="53"/>
       <c r="N16" s="2">
         <v>10</v>
+      </c>
+      <c r="O16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="P16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="Q16" s="12">
+        <v>44431</v>
+      </c>
+      <c r="R16" s="12">
+        <v>44431</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>11</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="10">
         <v>10</v>
       </c>
       <c r="C17" s="2">
         <v>11</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="10">
         <v>8</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="10">
         <v>4</v>
       </c>
       <c r="J17" s="57"/>
@@ -1737,6 +1769,15 @@
       <c r="M17" s="58"/>
       <c r="N17" s="2">
         <v>11</v>
+      </c>
+      <c r="O17" s="12">
+        <v>44432</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>44432</v>
+      </c>
+      <c r="R17" s="12">
+        <v>44432</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 12일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF017A-DF7A-42BF-9997-8259D567AEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6C585-0752-41A7-B135-F931B16422A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="60" windowWidth="26830" windowHeight="19720" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="1180" yWindow="930" windowWidth="27000" windowHeight="19720" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -206,6 +206,14 @@
   </si>
   <si>
     <t>다이나믹 프로그래밍 - 개념</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP - 1로 만들기, 개미전사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP - 바닥 공사, 효율적인 화폐 구성</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1122,7 +1130,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1754,7 +1762,7 @@
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="10">
         <v>11</v>
       </c>
       <c r="D17" s="10">
@@ -1763,15 +1771,26 @@
       <c r="E17" s="10">
         <v>4</v>
       </c>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="58"/>
+      <c r="H17" s="11">
+        <v>11</v>
+      </c>
+      <c r="I17" s="12">
+        <v>44433</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
       <c r="O17" s="12">
         <v>44432</v>
+      </c>
+      <c r="P17" s="12">
+        <v>44433</v>
       </c>
       <c r="Q17" s="12">
         <v>44432</v>
@@ -1784,24 +1803,44 @@
       <c r="A18" s="2">
         <v>12</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="10">
         <v>12</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="10">
         <v>9</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="10">
         <v>5</v>
       </c>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="58"/>
+      <c r="H18" s="11">
+        <v>12</v>
+      </c>
+      <c r="I18" s="12">
+        <v>44434</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
       <c r="N18" s="2">
         <v>12</v>
+      </c>
+      <c r="O18" s="12">
+        <v>44434</v>
+      </c>
+      <c r="P18" s="12">
+        <v>44436</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>44436</v>
+      </c>
+      <c r="R18" s="12">
+        <v>44436</v>
       </c>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 13일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6C585-0752-41A7-B135-F931B16422A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2885461-1A17-412A-A8DF-CACB9D24FE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="930" windowWidth="27000" windowHeight="19720" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -661,6 +661,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -670,7 +740,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -806,6 +876,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
@@ -1130,7 +1210,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1149,7 +1229,9 @@
     <col min="12" max="12" width="11.58203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="27.08203125" style="3" customWidth="1"/>
     <col min="14" max="15" width="11.58203125" style="2" customWidth="1"/>
-    <col min="16" max="46" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="59" bestFit="1" customWidth="1"/>
+    <col min="23" max="46" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="47" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -1254,6 +1336,7 @@
       <c r="S3" s="41"/>
       <c r="T3" s="41"/>
       <c r="U3" s="42"/>
+      <c r="V3" s="60"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="38" t="s">
@@ -1283,6 +1366,7 @@
       <c r="S4" s="44"/>
       <c r="T4" s="44"/>
       <c r="U4" s="45"/>
+      <c r="V4" s="61"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A5" s="17"/>
@@ -1324,6 +1408,7 @@
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
+      <c r="V5" s="59"/>
     </row>
     <row r="6" spans="1:36" s="9" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -1376,6 +1461,7 @@
       <c r="T6" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="V6" s="62"/>
     </row>
     <row r="7" spans="1:36" ht="39.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
@@ -1404,6 +1490,29 @@
       <c r="P7" s="12">
         <v>44417</v>
       </c>
+      <c r="V7" s="64">
+        <v>44416</v>
+      </c>
+      <c r="W7" s="65">
+        <v>44417</v>
+      </c>
+      <c r="X7" s="65">
+        <v>44418</v>
+      </c>
+      <c r="Y7" s="65">
+        <v>44419</v>
+      </c>
+      <c r="Z7" s="65">
+        <v>44420</v>
+      </c>
+      <c r="AA7" s="65">
+        <v>44421</v>
+      </c>
+      <c r="AB7" s="65">
+        <v>44422</v>
+      </c>
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="65"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
@@ -1437,6 +1546,11 @@
       <c r="P8" s="12">
         <v>44418</v>
       </c>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
@@ -1470,6 +1584,28 @@
       <c r="P9" s="12">
         <v>44419</v>
       </c>
+      <c r="V9" s="63">
+        <v>44423</v>
+      </c>
+      <c r="W9" s="66">
+        <v>44424</v>
+      </c>
+      <c r="X9" s="66">
+        <v>44425</v>
+      </c>
+      <c r="Y9" s="66">
+        <v>44426</v>
+      </c>
+      <c r="Z9" s="66">
+        <v>44427</v>
+      </c>
+      <c r="AA9" s="66">
+        <v>44428</v>
+      </c>
+      <c r="AB9" s="66">
+        <v>44429</v>
+      </c>
+      <c r="AC9" s="66"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
@@ -1508,6 +1644,12 @@
       <c r="Q10" s="12">
         <v>44421</v>
       </c>
+      <c r="V10" s="67"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
@@ -1546,6 +1688,27 @@
       <c r="Q11" s="12">
         <v>44424</v>
       </c>
+      <c r="V11" s="63">
+        <v>44430</v>
+      </c>
+      <c r="W11" s="66">
+        <v>44431</v>
+      </c>
+      <c r="X11" s="66">
+        <v>44432</v>
+      </c>
+      <c r="Y11" s="66">
+        <v>44433</v>
+      </c>
+      <c r="Z11" s="66">
+        <v>44434</v>
+      </c>
+      <c r="AA11" s="66">
+        <v>44435</v>
+      </c>
+      <c r="AB11" s="66">
+        <v>44436</v>
+      </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
@@ -1584,6 +1747,13 @@
       <c r="Q12" s="12">
         <v>44425</v>
       </c>
+      <c r="V12" s="67"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="68"/>
+      <c r="Y12" s="68"/>
+      <c r="Z12" s="68"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="68"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
@@ -1622,6 +1792,27 @@
       <c r="Q13" s="12">
         <v>44426</v>
       </c>
+      <c r="V13" s="63">
+        <v>44437</v>
+      </c>
+      <c r="W13" s="66">
+        <v>44438</v>
+      </c>
+      <c r="X13" s="66">
+        <v>44439</v>
+      </c>
+      <c r="Y13" s="66">
+        <v>44440</v>
+      </c>
+      <c r="Z13" s="66">
+        <v>44441</v>
+      </c>
+      <c r="AA13" s="66">
+        <v>44442</v>
+      </c>
+      <c r="AB13" s="66">
+        <v>44443</v>
+      </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
@@ -1666,6 +1857,13 @@
       <c r="R14" s="12">
         <v>44429</v>
       </c>
+      <c r="V14" s="67"/>
+      <c r="W14" s="68"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
@@ -1710,6 +1908,27 @@
       <c r="R15" s="12">
         <v>44430</v>
       </c>
+      <c r="V15" s="63">
+        <v>44444</v>
+      </c>
+      <c r="W15" s="66">
+        <v>44445</v>
+      </c>
+      <c r="X15" s="66">
+        <v>44446</v>
+      </c>
+      <c r="Y15" s="66">
+        <v>44447</v>
+      </c>
+      <c r="Z15" s="66">
+        <v>44448</v>
+      </c>
+      <c r="AA15" s="66">
+        <v>44449</v>
+      </c>
+      <c r="AB15" s="66">
+        <v>44450</v>
+      </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
@@ -1754,6 +1973,12 @@
       <c r="R16" s="12">
         <v>44431</v>
       </c>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
@@ -1798,6 +2023,27 @@
       <c r="R17" s="12">
         <v>44432</v>
       </c>
+      <c r="V17" s="63">
+        <v>44451</v>
+      </c>
+      <c r="W17" s="66">
+        <v>44452</v>
+      </c>
+      <c r="X17" s="66">
+        <v>44453</v>
+      </c>
+      <c r="Y17" s="66">
+        <v>44454</v>
+      </c>
+      <c r="Z17" s="66">
+        <v>44455</v>
+      </c>
+      <c r="AA17" s="66">
+        <v>44456</v>
+      </c>
+      <c r="AB17" s="66">
+        <v>44457</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
@@ -1843,23 +2089,35 @@
         <v>44436</v>
       </c>
       <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
+      <c r="V18" s="63"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>13</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="10">
         <v>12</v>
       </c>
       <c r="C19" s="2">
         <v>13</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="10">
         <v>10</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="10">
         <v>6</v>
+      </c>
+      <c r="H19" s="11">
+        <v>13</v>
+      </c>
+      <c r="I19" s="12">
+        <v>44438</v>
       </c>
       <c r="J19" s="57"/>
       <c r="K19" s="57"/>
@@ -1868,7 +2126,36 @@
       <c r="N19" s="2">
         <v>13</v>
       </c>
-      <c r="V19" s="12"/>
+      <c r="O19" s="12">
+        <v>44437</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>44438</v>
+      </c>
+      <c r="R19" s="12">
+        <v>44438</v>
+      </c>
+      <c r="V19" s="63">
+        <v>44458</v>
+      </c>
+      <c r="W19" s="66">
+        <v>44459</v>
+      </c>
+      <c r="X19" s="66">
+        <v>44460</v>
+      </c>
+      <c r="Y19" s="66">
+        <v>44461</v>
+      </c>
+      <c r="Z19" s="66">
+        <v>44462</v>
+      </c>
+      <c r="AA19" s="66">
+        <v>44463</v>
+      </c>
+      <c r="AB19" s="66">
+        <v>44464</v>
+      </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
@@ -1893,6 +2180,12 @@
       <c r="N20" s="2">
         <v>14</v>
       </c>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
@@ -1921,9 +2214,27 @@
         <v>15</v>
       </c>
       <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
+      <c r="V21" s="63">
+        <v>44465</v>
+      </c>
+      <c r="W21" s="66">
+        <v>44466</v>
+      </c>
+      <c r="X21" s="66">
+        <v>44467</v>
+      </c>
+      <c r="Y21" s="66">
+        <v>44468</v>
+      </c>
+      <c r="Z21" s="66">
+        <v>44469</v>
+      </c>
+      <c r="AA21" s="66">
+        <v>44470</v>
+      </c>
+      <c r="AB21" s="66">
+        <v>44471</v>
+      </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
@@ -1951,9 +2262,12 @@
       <c r="N22" s="2">
         <v>16</v>
       </c>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="66"/>
+      <c r="Y22" s="66"/>
+      <c r="Z22" s="66"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
@@ -1981,8 +2295,15 @@
       <c r="N23" s="2">
         <v>17</v>
       </c>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
+      <c r="V23" s="63">
+        <v>44472</v>
+      </c>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
@@ -2154,7 +2475,7 @@
         <v>23</v>
       </c>
       <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
+      <c r="V29" s="63"/>
       <c r="W29" s="12"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.45">
@@ -2752,7 +3073,7 @@
       <c r="N54" s="2">
         <v>48</v>
       </c>
-      <c r="V54" s="12"/>
+      <c r="V54" s="63"/>
       <c r="W54" s="12"/>
       <c r="AT54" s="12"/>
     </row>
@@ -2968,7 +3289,7 @@
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.45">
       <c r="U68" s="12"/>
-      <c r="V68" s="12"/>
+      <c r="V68" s="63"/>
       <c r="W68" s="12"/>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 14일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813C7EDA-07D9-482A-813D-84CBDFBA4632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EDAC-E540-470D-A816-1ED2CDAADBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -218,6 +218,10 @@
   </si>
   <si>
     <t>최단경로 - 다익스트라, 플로이드 워셜 알고리즘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>최단경로 - 미래도시, 전보</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -800,95 +804,95 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1214,7 +1218,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1240,113 +1244,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68" t="s">
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="63"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:36" s="6" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="48"/>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="23" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="47" t="s">
+      <c r="N3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="49"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="52"/>
       <c r="V3" s="30"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1359,17 +1363,17 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="52"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="54"/>
+      <c r="U4" s="55"/>
       <c r="V4" s="31"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
@@ -1392,15 +1396,15 @@
       <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="53" t="s">
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="54"/>
+      <c r="L5" s="57"/>
       <c r="M5" s="25" t="s">
         <v>32</v>
       </c>
@@ -1436,14 +1440,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1482,12 +1486,12 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="58" t="s">
+      <c r="J7" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="42"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1535,12 +1539,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="42"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="47"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1573,12 +1577,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1630,12 +1634,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="42"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="47"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1674,12 +1678,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="42"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="47"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1778,12 +1782,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1863,7 +1867,7 @@
       </c>
       <c r="V14" s="37"/>
       <c r="W14" s="38"/>
-      <c r="X14" s="15"/>
+      <c r="X14" s="38"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
       <c r="AA14" s="15"/>
@@ -1891,12 +1895,12 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="42"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="47"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -1956,12 +1960,12 @@
       <c r="I16" s="12">
         <v>44431</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -2006,12 +2010,12 @@
       <c r="I17" s="12">
         <v>44433</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="42"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="47"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -2071,12 +2075,12 @@
       <c r="I18" s="12">
         <v>44434</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="J18" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="42"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="47"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -2123,12 +2127,12 @@
       <c r="I19" s="12">
         <v>44438</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -2170,24 +2174,44 @@
       <c r="A20" s="2">
         <v>14</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="10">
         <v>14</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="10">
         <v>11</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="10">
         <v>7</v>
       </c>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="40"/>
+      <c r="H20" s="11">
+        <v>14</v>
+      </c>
+      <c r="I20" s="12">
+        <v>44439</v>
+      </c>
+      <c r="J20" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
       <c r="N20" s="2">
         <v>14</v>
+      </c>
+      <c r="O20" s="12">
+        <v>44439</v>
+      </c>
+      <c r="P20" s="12">
+        <v>44439</v>
+      </c>
+      <c r="Q20" s="12">
+        <v>44439</v>
+      </c>
+      <c r="R20" s="12">
+        <v>44439</v>
       </c>
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
@@ -2215,10 +2239,10 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="68"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -2264,10 +2288,10 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="40"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="68"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -2297,10 +2321,10 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="40"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="68"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -2333,10 +2357,10 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="68"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -2362,10 +2386,10 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="68"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -2390,10 +2414,10 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="40"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="68"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -2419,10 +2443,10 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="40"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="68"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2448,16 +2472,16 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="40"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="68"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
       <c r="AC28" s="12"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>23</v>
       </c>
@@ -2476,10 +2500,10 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="68"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -2506,10 +2530,10 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="40"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="68"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2536,10 +2560,10 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="40"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="68"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2566,10 +2590,10 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="40"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="68"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2596,10 +2620,10 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="40"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="68"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2626,10 +2650,10 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="40"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="68"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2656,10 +2680,10 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="40"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="68"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2686,10 +2710,10 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="40"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="68"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2716,10 +2740,10 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="40"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="68"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2742,10 +2766,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="40"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="68"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2767,10 +2791,10 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="40"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="68"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2789,10 +2813,10 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="40"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="68"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2812,10 +2836,10 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="40"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="68"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2836,10 +2860,10 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="40"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="68"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2860,10 +2884,10 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="40"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="68"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2880,10 +2904,10 @@
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="40"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
+      <c r="M44" s="68"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2901,10 +2925,10 @@
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="40"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="68"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2922,10 +2946,10 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="40"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="68"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2942,10 +2966,10 @@
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="40"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="67"/>
+      <c r="M47" s="68"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -2962,10 +2986,10 @@
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="40"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
+      <c r="M48" s="68"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -2982,10 +3006,10 @@
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="40"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="67"/>
+      <c r="M49" s="68"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -3003,10 +3027,10 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="40"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="68"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -3021,10 +3045,10 @@
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="40"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="67"/>
+      <c r="M51" s="68"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -3039,10 +3063,10 @@
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="40"/>
+      <c r="J52" s="67"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="67"/>
+      <c r="M52" s="68"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -3057,10 +3081,10 @@
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="40"/>
+      <c r="J53" s="67"/>
+      <c r="K53" s="67"/>
+      <c r="L53" s="67"/>
+      <c r="M53" s="68"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -3075,10 +3099,10 @@
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="40"/>
+      <c r="J54" s="67"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="67"/>
+      <c r="M54" s="68"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -3093,10 +3117,10 @@
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="40"/>
+      <c r="J55" s="67"/>
+      <c r="K55" s="67"/>
+      <c r="L55" s="67"/>
+      <c r="M55" s="68"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -3111,10 +3135,10 @@
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="40"/>
+      <c r="J56" s="67"/>
+      <c r="K56" s="67"/>
+      <c r="L56" s="67"/>
+      <c r="M56" s="68"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -3129,10 +3153,10 @@
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="40"/>
+      <c r="J57" s="67"/>
+      <c r="K57" s="67"/>
+      <c r="L57" s="67"/>
+      <c r="M57" s="68"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -3147,10 +3171,10 @@
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="40"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="67"/>
+      <c r="M58" s="68"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -3165,10 +3189,10 @@
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="40"/>
+      <c r="J59" s="67"/>
+      <c r="K59" s="67"/>
+      <c r="L59" s="67"/>
+      <c r="M59" s="68"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -3183,10 +3207,10 @@
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="40"/>
+      <c r="J60" s="67"/>
+      <c r="K60" s="67"/>
+      <c r="L60" s="67"/>
+      <c r="M60" s="68"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -3199,10 +3223,10 @@
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="40"/>
+      <c r="J61" s="67"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="67"/>
+      <c r="M61" s="68"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -3218,10 +3242,10 @@
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="40"/>
+      <c r="J62" s="67"/>
+      <c r="K62" s="67"/>
+      <c r="L62" s="67"/>
+      <c r="M62" s="68"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -3236,10 +3260,10 @@
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
-      <c r="M63" s="40"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="67"/>
+      <c r="M63" s="68"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -3254,10 +3278,10 @@
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="40"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="67"/>
+      <c r="L64" s="67"/>
+      <c r="M64" s="68"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -3271,10 +3295,10 @@
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="40"/>
+      <c r="J65" s="67"/>
+      <c r="K65" s="67"/>
+      <c r="L65" s="67"/>
+      <c r="M65" s="68"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -3283,10 +3307,10 @@
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="40"/>
+      <c r="J66" s="67"/>
+      <c r="K66" s="67"/>
+      <c r="L66" s="67"/>
+      <c r="M66" s="68"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -3364,18 +3388,59 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
@@ -3390,59 +3455,18 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 15일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EDAC-E540-470D-A816-1ED2CDAADBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F1CB1F-244F-4F06-9838-FDF2AF065167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="1020" yWindow="3000" windowWidth="29780" windowHeight="17120" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -804,6 +804,75 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,75 +893,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61086F-FA6B-47FC-85D4-709DD8996956}">
   <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1244,113 +1244,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45" t="s">
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45" t="s">
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45" t="s">
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39" t="s">
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="63"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:36" s="6" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="45"/>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
       <c r="H3" s="23" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="50" t="s">
+      <c r="N3" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="52"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="49"/>
       <c r="V3" s="30"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1363,17 +1363,17 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="55"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="52"/>
       <c r="V4" s="31"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
@@ -1396,15 +1396,15 @@
       <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="56" t="s">
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="57"/>
+      <c r="L5" s="54"/>
       <c r="M5" s="25" t="s">
         <v>32</v>
       </c>
@@ -1440,14 +1440,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="60"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1486,12 +1486,12 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="61" t="s">
+      <c r="J7" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="42"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1539,12 +1539,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="47"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="42"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1577,12 +1577,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="63"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1634,12 +1634,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="47"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="42"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1678,12 +1678,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="47"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="42"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1782,12 +1782,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="46" t="s">
+      <c r="J13" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="42"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1895,12 +1895,12 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="46" t="s">
+      <c r="J15" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="47"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="42"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -1960,12 +1960,12 @@
       <c r="I16" s="12">
         <v>44431</v>
       </c>
-      <c r="J16" s="62" t="s">
+      <c r="J16" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="63"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="44"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -2010,12 +2010,12 @@
       <c r="I17" s="12">
         <v>44433</v>
       </c>
-      <c r="J17" s="46" t="s">
+      <c r="J17" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="42"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -2075,12 +2075,12 @@
       <c r="I18" s="12">
         <v>44434</v>
       </c>
-      <c r="J18" s="46" t="s">
+      <c r="J18" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="47"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="42"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -2127,12 +2127,12 @@
       <c r="I19" s="12">
         <v>44438</v>
       </c>
-      <c r="J19" s="62" t="s">
+      <c r="J19" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="63"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -2192,12 +2192,12 @@
       <c r="I20" s="12">
         <v>44439</v>
       </c>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="42"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -2224,27 +2224,39 @@
       <c r="A21" s="2">
         <v>15</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="10">
         <v>14</v>
       </c>
       <c r="C21" s="2">
         <v>15</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="10">
         <v>12</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="10">
         <v>8</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="10">
         <v>1</v>
       </c>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="68"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="40"/>
       <c r="N21" s="2">
         <v>15</v>
+      </c>
+      <c r="O21" s="12">
+        <v>44440</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>44440</v>
+      </c>
+      <c r="R21" s="12">
+        <v>44440</v>
+      </c>
+      <c r="S21" s="12">
+        <v>44440</v>
       </c>
       <c r="U21" s="12"/>
       <c r="V21" s="33">
@@ -2288,10 +2300,10 @@
       <c r="F22" s="2">
         <v>2</v>
       </c>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="68"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="40"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -2321,10 +2333,10 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="68"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="40"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -2357,10 +2369,10 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="68"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="40"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -2386,10 +2398,10 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="68"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="40"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -2414,10 +2426,10 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="68"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="40"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -2443,10 +2455,10 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="40"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2472,10 +2484,10 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="68"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="40"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -2500,10 +2512,10 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="68"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="40"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -2530,10 +2542,10 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="68"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="40"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2560,10 +2572,10 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="68"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="40"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2590,10 +2602,10 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="68"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="40"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2620,10 +2632,10 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="68"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="40"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2650,10 +2662,10 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="68"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="40"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2680,10 +2692,10 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="68"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="40"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2710,10 +2722,10 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="67"/>
-      <c r="K36" s="67"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="68"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="40"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2740,10 +2752,10 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="67"/>
-      <c r="K37" s="67"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="68"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="40"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2766,10 +2778,10 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="68"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="40"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2791,10 +2803,10 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="68"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="40"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2813,10 +2825,10 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="67"/>
-      <c r="K40" s="67"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="68"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="40"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2836,10 +2848,10 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="67"/>
-      <c r="K41" s="67"/>
-      <c r="L41" s="67"/>
-      <c r="M41" s="68"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="40"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2860,10 +2872,10 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="67"/>
-      <c r="K42" s="67"/>
-      <c r="L42" s="67"/>
-      <c r="M42" s="68"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="40"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2884,10 +2896,10 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="67"/>
-      <c r="K43" s="67"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="68"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="40"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2904,10 +2916,10 @@
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="67"/>
-      <c r="K44" s="67"/>
-      <c r="L44" s="67"/>
-      <c r="M44" s="68"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="40"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2925,10 +2937,10 @@
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="67"/>
-      <c r="K45" s="67"/>
-      <c r="L45" s="67"/>
-      <c r="M45" s="68"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="40"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2946,10 +2958,10 @@
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
-      <c r="L46" s="67"/>
-      <c r="M46" s="68"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="40"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2966,10 +2978,10 @@
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="67"/>
-      <c r="K47" s="67"/>
-      <c r="L47" s="67"/>
-      <c r="M47" s="68"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="40"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -2986,10 +2998,10 @@
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="67"/>
-      <c r="K48" s="67"/>
-      <c r="L48" s="67"/>
-      <c r="M48" s="68"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="40"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -3006,10 +3018,10 @@
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="67"/>
-      <c r="K49" s="67"/>
-      <c r="L49" s="67"/>
-      <c r="M49" s="68"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="40"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -3027,10 +3039,10 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="67"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="67"/>
-      <c r="M50" s="68"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="40"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -3045,10 +3057,10 @@
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67"/>
-      <c r="L51" s="67"/>
-      <c r="M51" s="68"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="40"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -3063,10 +3075,10 @@
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="67"/>
-      <c r="K52" s="67"/>
-      <c r="L52" s="67"/>
-      <c r="M52" s="68"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="40"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -3081,10 +3093,10 @@
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="67"/>
-      <c r="K53" s="67"/>
-      <c r="L53" s="67"/>
-      <c r="M53" s="68"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="39"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="40"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -3099,10 +3111,10 @@
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="67"/>
-      <c r="K54" s="67"/>
-      <c r="L54" s="67"/>
-      <c r="M54" s="68"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="40"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -3117,10 +3129,10 @@
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="67"/>
-      <c r="K55" s="67"/>
-      <c r="L55" s="67"/>
-      <c r="M55" s="68"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="40"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -3135,10 +3147,10 @@
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="67"/>
-      <c r="K56" s="67"/>
-      <c r="L56" s="67"/>
-      <c r="M56" s="68"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="40"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -3153,10 +3165,10 @@
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="67"/>
-      <c r="K57" s="67"/>
-      <c r="L57" s="67"/>
-      <c r="M57" s="68"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="39"/>
+      <c r="M57" s="40"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -3171,10 +3183,10 @@
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="67"/>
-      <c r="K58" s="67"/>
-      <c r="L58" s="67"/>
-      <c r="M58" s="68"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="40"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -3189,10 +3201,10 @@
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="67"/>
-      <c r="K59" s="67"/>
-      <c r="L59" s="67"/>
-      <c r="M59" s="68"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="39"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="40"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -3207,10 +3219,10 @@
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="67"/>
-      <c r="K60" s="67"/>
-      <c r="L60" s="67"/>
-      <c r="M60" s="68"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="40"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -3223,10 +3235,10 @@
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="67"/>
-      <c r="K61" s="67"/>
-      <c r="L61" s="67"/>
-      <c r="M61" s="68"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="40"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -3242,10 +3254,10 @@
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="67"/>
-      <c r="K62" s="67"/>
-      <c r="L62" s="67"/>
-      <c r="M62" s="68"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="40"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -3260,10 +3272,10 @@
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="67"/>
-      <c r="K63" s="67"/>
-      <c r="L63" s="67"/>
-      <c r="M63" s="68"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="40"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -3278,10 +3290,10 @@
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="67"/>
-      <c r="K64" s="67"/>
-      <c r="L64" s="67"/>
-      <c r="M64" s="68"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="39"/>
+      <c r="L64" s="39"/>
+      <c r="M64" s="40"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -3295,10 +3307,10 @@
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="67"/>
-      <c r="K65" s="67"/>
-      <c r="L65" s="67"/>
-      <c r="M65" s="68"/>
+      <c r="J65" s="39"/>
+      <c r="K65" s="39"/>
+      <c r="L65" s="39"/>
+      <c r="M65" s="40"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -3307,10 +3319,10 @@
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="67"/>
-      <c r="K66" s="67"/>
-      <c r="L66" s="67"/>
-      <c r="M66" s="68"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="39"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="40"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -3388,59 +3400,18 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
@@ -3455,18 +3426,59 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 16일차
- 그래프 이론 개념 : 다시 봄
- 최단 경로 개념 (다익스트라, 플로이드 워셜) : 다시 봄
- 이진 탐색 문제 - 떡볶이 떡 만들기 : 다시 풀음
- 구현 문제 - 왕실의 나이트, 게임 개발 : 다시 풀음
  - 카카오 문제를 풀면서 느낀게, 알고리즘 문제가 딱 하나의 알고리즘으로만 풀리는게 아니라는 것이다. 그래서 예전에 풀고 복습으로 다시 푸는 문제들을 새로 알게된 방식으로 풀어보려고 노력한다. 게임 개발의 경우 구현으로 풀 수 있지만, DFS, BFS로도 풀 수 있다. 이렇게 한 문제를 여러 알고리즘으로 풀어보면, 내가 알고리즘을 얼마나 알고 있는지 확인 할 수 있고, 성장의 폭이 커지지 않을까/
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F1CB1F-244F-4F06-9838-FDF2AF065167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295647DF-B5F9-4D09-8D4E-760470548944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="3000" windowWidth="29780" windowHeight="17120" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="1080" yWindow="2690" windowWidth="29780" windowHeight="17120" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -222,6 +222,10 @@
   </si>
   <si>
     <t>최단경로 - 미래도시, 전보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래프 이론 - 1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1218,7 +1222,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2227,7 +2231,7 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="10">
         <v>15</v>
       </c>
       <c r="D21" s="10">
@@ -2239,14 +2243,25 @@
       <c r="F21" s="10">
         <v>1</v>
       </c>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
+      <c r="H21" s="11">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12">
+        <v>44440</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
       <c r="O21" s="12">
+        <v>44440</v>
+      </c>
+      <c r="P21" s="12">
         <v>44440</v>
       </c>
       <c r="Q21" s="12">
@@ -2285,19 +2300,19 @@
       <c r="A22" s="2">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="10">
         <v>15</v>
       </c>
       <c r="C22" s="2">
         <v>16</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="10">
         <v>13</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="10">
         <v>9</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="10">
         <v>2</v>
       </c>
       <c r="J22" s="39"/>
@@ -2306,6 +2321,18 @@
       <c r="M22" s="40"/>
       <c r="N22" s="2">
         <v>16</v>
+      </c>
+      <c r="O22" s="12">
+        <v>44441</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>44441</v>
+      </c>
+      <c r="R22" s="12">
+        <v>44441</v>
+      </c>
+      <c r="S22" s="12">
+        <v>44441</v>
       </c>
       <c r="W22" s="15"/>
       <c r="X22" s="36"/>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 17일차
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295647DF-B5F9-4D09-8D4E-760470548944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB394B-3984-44D3-BE44-7330EA61457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2690" windowWidth="29780" windowHeight="17120" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="680" yWindow="640" windowWidth="23200" windowHeight="20360" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>그래프 이론 - 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래프 이론 - 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>알고리즘 &amp; SQL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래프 - 팀 결성, 도시 분할 계획</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -277,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,8 +337,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -743,6 +761,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -752,7 +844,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -788,7 +880,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,6 +899,8 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -829,6 +922,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,6 +985,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,6 +1010,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1221,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61086F-FA6B-47FC-85D4-709DD8996956}">
   <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1242,119 +1359,122 @@
     <col min="13" max="13" width="27.08203125" style="3" customWidth="1"/>
     <col min="14" max="15" width="11.58203125" style="2" customWidth="1"/>
     <col min="16" max="21" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="28" bestFit="1" customWidth="1"/>
     <col min="23" max="46" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="47" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68" t="s">
+      <c r="E1" s="76"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68" t="s">
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68" t="s">
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="63"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="67"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:36" s="6" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:36" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="23" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="38" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="47" t="s">
+      <c r="N3" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="30"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="29"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1362,27 +1482,27 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="31"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="30"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A5" s="17"/>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -1400,16 +1520,16 @@
       <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="53" t="s">
+      <c r="I5" s="62"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="25" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="24" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="16"/>
@@ -1420,7 +1540,7 @@
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
-      <c r="V5" s="29"/>
+      <c r="V5" s="28"/>
     </row>
     <row r="6" spans="1:36" s="9" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
@@ -1444,14 +1564,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="59"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1593,7 @@
       <c r="T6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="32"/>
+      <c r="V6" s="31"/>
     </row>
     <row r="7" spans="1:36" ht="39.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
@@ -1490,41 +1610,41 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="58" t="s">
+      <c r="J7" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
       <c r="P7" s="12">
         <v>44417</v>
       </c>
-      <c r="V7" s="34">
+      <c r="V7" s="33">
         <v>44416</v>
       </c>
-      <c r="W7" s="35">
+      <c r="W7" s="34">
         <v>44417</v>
       </c>
-      <c r="X7" s="35">
+      <c r="X7" s="34">
         <v>44418</v>
       </c>
-      <c r="Y7" s="35">
+      <c r="Y7" s="34">
         <v>44419</v>
       </c>
-      <c r="Z7" s="35">
+      <c r="Z7" s="34">
         <v>44420</v>
       </c>
-      <c r="AA7" s="35">
+      <c r="AA7" s="34">
         <v>44421</v>
       </c>
-      <c r="AB7" s="35">
+      <c r="AB7" s="34">
         <v>44422</v>
       </c>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="35"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
@@ -1543,12 +1663,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="43"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1581,12 +1701,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1596,28 +1716,28 @@
       <c r="P9" s="12">
         <v>44419</v>
       </c>
-      <c r="V9" s="33">
+      <c r="V9" s="32">
         <v>44423</v>
       </c>
-      <c r="W9" s="36">
+      <c r="W9" s="35">
         <v>44424</v>
       </c>
-      <c r="X9" s="36">
+      <c r="X9" s="35">
         <v>44425</v>
       </c>
-      <c r="Y9" s="36">
+      <c r="Y9" s="35">
         <v>44426</v>
       </c>
-      <c r="Z9" s="36">
+      <c r="Z9" s="35">
         <v>44427</v>
       </c>
-      <c r="AA9" s="36">
+      <c r="AA9" s="35">
         <v>44428</v>
       </c>
-      <c r="AB9" s="36">
+      <c r="AB9" s="35">
         <v>44429</v>
       </c>
-      <c r="AC9" s="36"/>
+      <c r="AC9" s="35"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
@@ -1638,12 +1758,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1656,7 +1776,7 @@
       <c r="Q10" s="12">
         <v>44421</v>
       </c>
-      <c r="V10" s="37"/>
+      <c r="V10" s="36"/>
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
@@ -1682,12 +1802,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1700,25 +1820,25 @@
       <c r="Q11" s="12">
         <v>44424</v>
       </c>
-      <c r="V11" s="33">
+      <c r="V11" s="32">
         <v>44430</v>
       </c>
-      <c r="W11" s="36">
+      <c r="W11" s="35">
         <v>44431</v>
       </c>
-      <c r="X11" s="36">
+      <c r="X11" s="35">
         <v>44432</v>
       </c>
-      <c r="Y11" s="36">
+      <c r="Y11" s="35">
         <v>44433</v>
       </c>
-      <c r="Z11" s="36">
+      <c r="Z11" s="35">
         <v>44434</v>
       </c>
-      <c r="AA11" s="36">
+      <c r="AA11" s="35">
         <v>44435</v>
       </c>
-      <c r="AB11" s="36">
+      <c r="AB11" s="35">
         <v>44436</v>
       </c>
     </row>
@@ -1741,12 +1861,12 @@
       <c r="I12" s="12">
         <v>44425</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="25"/>
       <c r="N12" s="2">
         <v>6</v>
       </c>
@@ -1759,13 +1879,13 @@
       <c r="Q12" s="12">
         <v>44425</v>
       </c>
-      <c r="V12" s="37"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="38"/>
+      <c r="AB12" s="37"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
@@ -1786,12 +1906,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1804,25 +1924,25 @@
       <c r="Q13" s="12">
         <v>44426</v>
       </c>
-      <c r="V13" s="33">
+      <c r="V13" s="32">
         <v>44437</v>
       </c>
-      <c r="W13" s="36">
+      <c r="W13" s="35">
         <v>44438</v>
       </c>
-      <c r="X13" s="36">
+      <c r="X13" s="35">
         <v>44439</v>
       </c>
-      <c r="Y13" s="36">
+      <c r="Y13" s="35">
         <v>44440</v>
       </c>
-      <c r="Z13" s="36">
+      <c r="Z13" s="35">
         <v>44441</v>
       </c>
-      <c r="AA13" s="36">
+      <c r="AA13" s="35">
         <v>44442</v>
       </c>
-      <c r="AB13" s="36">
+      <c r="AB13" s="35">
         <v>44443</v>
       </c>
     </row>
@@ -1848,12 +1968,12 @@
       <c r="I14" s="12">
         <v>44428</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="25"/>
       <c r="N14" s="2">
         <v>8</v>
       </c>
@@ -1869,12 +1989,12 @@
       <c r="R14" s="12">
         <v>44429</v>
       </c>
-      <c r="V14" s="37"/>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="37"/>
       <c r="AB14" s="15"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.45">
@@ -1899,12 +2019,12 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="43"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -1920,25 +2040,25 @@
       <c r="R15" s="12">
         <v>44430</v>
       </c>
-      <c r="V15" s="33">
+      <c r="V15" s="32">
         <v>44444</v>
       </c>
-      <c r="W15" s="36">
+      <c r="W15" s="35">
         <v>44445</v>
       </c>
-      <c r="X15" s="36">
+      <c r="X15" s="35">
         <v>44446</v>
       </c>
-      <c r="Y15" s="36">
+      <c r="Y15" s="35">
         <v>44447</v>
       </c>
-      <c r="Z15" s="36">
+      <c r="Z15" s="35">
         <v>44448</v>
       </c>
-      <c r="AA15" s="36">
+      <c r="AA15" s="35">
         <v>44449</v>
       </c>
-      <c r="AB15" s="36">
+      <c r="AB15" s="35">
         <v>44450</v>
       </c>
     </row>
@@ -1964,12 +2084,12 @@
       <c r="I16" s="12">
         <v>44431</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -2014,12 +2134,12 @@
       <c r="I17" s="12">
         <v>44433</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="J17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -2035,25 +2155,25 @@
       <c r="R17" s="12">
         <v>44432</v>
       </c>
-      <c r="V17" s="33">
+      <c r="V17" s="32">
         <v>44451</v>
       </c>
-      <c r="W17" s="36">
+      <c r="W17" s="35">
         <v>44452</v>
       </c>
-      <c r="X17" s="36">
+      <c r="X17" s="35">
         <v>44453</v>
       </c>
-      <c r="Y17" s="36">
+      <c r="Y17" s="35">
         <v>44454</v>
       </c>
-      <c r="Z17" s="36">
+      <c r="Z17" s="35">
         <v>44455</v>
       </c>
-      <c r="AA17" s="36">
+      <c r="AA17" s="35">
         <v>44456</v>
       </c>
-      <c r="AB17" s="36">
+      <c r="AB17" s="35">
         <v>44457</v>
       </c>
     </row>
@@ -2079,12 +2199,12 @@
       <c r="I18" s="12">
         <v>44434</v>
       </c>
-      <c r="J18" s="41" t="s">
+      <c r="J18" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="43"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -2101,7 +2221,7 @@
         <v>44436</v>
       </c>
       <c r="U18" s="12"/>
-      <c r="V18" s="33"/>
+      <c r="V18" s="32"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
@@ -2131,12 +2251,12 @@
       <c r="I19" s="12">
         <v>44438</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -2152,25 +2272,25 @@
       <c r="R19" s="12">
         <v>44438</v>
       </c>
-      <c r="V19" s="33">
+      <c r="V19" s="32">
         <v>44458</v>
       </c>
-      <c r="W19" s="36">
+      <c r="W19" s="35">
         <v>44459</v>
       </c>
-      <c r="X19" s="36">
+      <c r="X19" s="35">
         <v>44460</v>
       </c>
-      <c r="Y19" s="36">
+      <c r="Y19" s="35">
         <v>44461</v>
       </c>
-      <c r="Z19" s="36">
+      <c r="Z19" s="35">
         <v>44462</v>
       </c>
-      <c r="AA19" s="36">
+      <c r="AA19" s="35">
         <v>44463</v>
       </c>
-      <c r="AB19" s="36">
+      <c r="AB19" s="35">
         <v>44464</v>
       </c>
     </row>
@@ -2196,12 +2316,12 @@
       <c r="I20" s="12">
         <v>44439</v>
       </c>
-      <c r="J20" s="41" t="s">
+      <c r="J20" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="43"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -2249,12 +2369,12 @@
       <c r="I21" s="12">
         <v>44440</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="45"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -2274,25 +2394,25 @@
         <v>44440</v>
       </c>
       <c r="U21" s="12"/>
-      <c r="V21" s="33">
+      <c r="V21" s="32">
         <v>44465</v>
       </c>
-      <c r="W21" s="36">
+      <c r="W21" s="35">
         <v>44466</v>
       </c>
-      <c r="X21" s="36">
+      <c r="X21" s="35">
         <v>44467</v>
       </c>
-      <c r="Y21" s="36">
+      <c r="Y21" s="35">
         <v>44468</v>
       </c>
-      <c r="Z21" s="36">
+      <c r="Z21" s="35">
         <v>44469</v>
       </c>
-      <c r="AA21" s="36">
+      <c r="AA21" s="35">
         <v>44470</v>
       </c>
-      <c r="AB21" s="36">
+      <c r="AB21" s="35">
         <v>44471</v>
       </c>
     </row>
@@ -2303,7 +2423,7 @@
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="10">
         <v>16</v>
       </c>
       <c r="D22" s="10">
@@ -2315,16 +2435,27 @@
       <c r="F22" s="10">
         <v>2</v>
       </c>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="40"/>
+      <c r="H22" s="11">
+        <v>16</v>
+      </c>
+      <c r="I22" s="12">
+        <v>44441</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
       <c r="O22" s="12">
         <v>44441</v>
       </c>
+      <c r="P22" s="12">
+        <v>44441</v>
+      </c>
       <c r="Q22" s="12">
         <v>44441</v>
       </c>
@@ -2335,9 +2466,9 @@
         <v>44441</v>
       </c>
       <c r="W22" s="15"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
       <c r="AA22" s="15"/>
       <c r="AB22" s="15"/>
     </row>
@@ -2345,35 +2476,58 @@
       <c r="A23" s="2">
         <v>17</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="10">
         <v>17</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="10">
         <v>14</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="10">
         <v>10</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="10">
         <v>3</v>
       </c>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="40"/>
+      <c r="H23" s="11">
+        <v>17</v>
+      </c>
+      <c r="I23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
-      <c r="V23" s="33">
+      <c r="O23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="P23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="Q23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="R23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="S23" s="12">
+        <v>44442</v>
+      </c>
+      <c r="V23" s="32">
         <v>44472</v>
       </c>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
+      <c r="Y23" s="35"/>
+      <c r="Z23" s="35"/>
       <c r="AA23" s="15"/>
       <c r="AB23" s="15"/>
     </row>
@@ -2396,10 +2550,16 @@
       <c r="F24" s="2">
         <v>4</v>
       </c>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="40"/>
+      <c r="H24" s="11">
+        <v>18</v>
+      </c>
+      <c r="I24" s="12">
+        <v>44443</v>
+      </c>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
       <c r="N24" s="2">
         <v>18</v>
       </c>
@@ -2425,10 +2585,16 @@
       <c r="F25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
+      <c r="H25" s="11">
+        <v>19</v>
+      </c>
+      <c r="I25" s="12">
+        <v>44444</v>
+      </c>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="41"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -2453,10 +2619,16 @@
       <c r="F26" s="2">
         <v>6</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="40"/>
+      <c r="H26" s="11">
+        <v>20</v>
+      </c>
+      <c r="I26" s="12">
+        <v>44445</v>
+      </c>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -2482,10 +2654,16 @@
       <c r="F27" s="2">
         <v>7</v>
       </c>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="40"/>
+      <c r="H27" s="11">
+        <v>21</v>
+      </c>
+      <c r="I27" s="12">
+        <v>44446</v>
+      </c>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="41"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2511,10 +2689,16 @@
       <c r="F28" s="2">
         <v>8</v>
       </c>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="40"/>
+      <c r="H28" s="11">
+        <v>22</v>
+      </c>
+      <c r="I28" s="12">
+        <v>44447</v>
+      </c>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="41"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -2539,15 +2723,21 @@
       <c r="F29" s="2">
         <v>9</v>
       </c>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
+      <c r="H29" s="11">
+        <v>23</v>
+      </c>
+      <c r="I29" s="12">
+        <v>44448</v>
+      </c>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
       <c r="U29" s="12"/>
-      <c r="V29" s="33"/>
+      <c r="V29" s="32"/>
       <c r="W29" s="12"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.45">
@@ -2569,10 +2759,16 @@
       <c r="F30" s="2">
         <v>10</v>
       </c>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="40"/>
+      <c r="H30" s="11">
+        <v>24</v>
+      </c>
+      <c r="I30" s="12">
+        <v>44449</v>
+      </c>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="41"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2599,10 +2795,16 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="40"/>
+      <c r="H31" s="11">
+        <v>25</v>
+      </c>
+      <c r="I31" s="12">
+        <v>44450</v>
+      </c>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="41"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2629,10 +2831,16 @@
       <c r="F32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="40"/>
+      <c r="H32" s="11">
+        <v>26</v>
+      </c>
+      <c r="I32" s="12">
+        <v>44451</v>
+      </c>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="41"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2659,10 +2867,16 @@
       <c r="F33" s="2">
         <v>13</v>
       </c>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="40"/>
+      <c r="H33" s="11">
+        <v>27</v>
+      </c>
+      <c r="I33" s="12">
+        <v>44452</v>
+      </c>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="41"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2689,10 +2903,16 @@
       <c r="F34" s="2">
         <v>14</v>
       </c>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="40"/>
+      <c r="H34" s="11">
+        <v>28</v>
+      </c>
+      <c r="I34" s="12">
+        <v>44453</v>
+      </c>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2719,10 +2939,16 @@
       <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="40"/>
+      <c r="H35" s="11">
+        <v>29</v>
+      </c>
+      <c r="I35" s="12">
+        <v>44454</v>
+      </c>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2749,10 +2975,16 @@
       <c r="F36" s="2">
         <v>16</v>
       </c>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="40"/>
+      <c r="H36" s="11">
+        <v>30</v>
+      </c>
+      <c r="I36" s="12">
+        <v>44455</v>
+      </c>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="41"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -2767,6 +2999,9 @@
       <c r="B37" s="2">
         <v>30</v>
       </c>
+      <c r="C37" s="2">
+        <v>31</v>
+      </c>
       <c r="D37" s="2">
         <v>28</v>
       </c>
@@ -2779,10 +3014,16 @@
       <c r="G37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="40"/>
+      <c r="H37" s="11">
+        <v>31</v>
+      </c>
+      <c r="I37" s="12">
+        <v>44456</v>
+      </c>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="41"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -2793,6 +3034,12 @@
       <c r="A38" s="2">
         <v>32</v>
       </c>
+      <c r="B38" s="2">
+        <v>31</v>
+      </c>
+      <c r="C38" s="2">
+        <v>32</v>
+      </c>
       <c r="D38" s="2">
         <v>29</v>
       </c>
@@ -2805,10 +3052,16 @@
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="40"/>
+      <c r="H38" s="11">
+        <v>32</v>
+      </c>
+      <c r="I38" s="12">
+        <v>44457</v>
+      </c>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -2818,6 +3071,12 @@
       <c r="A39" s="2">
         <v>33</v>
       </c>
+      <c r="B39" s="2">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2">
+        <v>33</v>
+      </c>
       <c r="D39" s="2">
         <v>30</v>
       </c>
@@ -2830,10 +3089,16 @@
       <c r="G39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="40"/>
+      <c r="H39" s="11">
+        <v>33</v>
+      </c>
+      <c r="I39" s="12">
+        <v>44458</v>
+      </c>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="41"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -2843,6 +3108,15 @@
       <c r="A40" s="2">
         <v>34</v>
       </c>
+      <c r="B40" s="2">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2">
+        <v>34</v>
+      </c>
+      <c r="D40" s="2">
+        <v>31</v>
+      </c>
       <c r="E40" s="2">
         <v>27</v>
       </c>
@@ -2852,10 +3126,16 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="40"/>
+      <c r="H40" s="11">
+        <v>34</v>
+      </c>
+      <c r="I40" s="12">
+        <v>44459</v>
+      </c>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="41"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -2866,6 +3146,15 @@
       <c r="A41" s="2">
         <v>35</v>
       </c>
+      <c r="B41" s="2">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2">
+        <v>35</v>
+      </c>
+      <c r="D41" s="2">
+        <v>32</v>
+      </c>
       <c r="E41" s="2">
         <v>28</v>
       </c>
@@ -2875,10 +3164,16 @@
       <c r="G41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="40"/>
+      <c r="H41" s="11">
+        <v>35</v>
+      </c>
+      <c r="I41" s="12">
+        <v>44460</v>
+      </c>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="41"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -2890,6 +3185,15 @@
       <c r="A42" s="2">
         <v>36</v>
       </c>
+      <c r="B42" s="2">
+        <v>35</v>
+      </c>
+      <c r="C42" s="2">
+        <v>36</v>
+      </c>
+      <c r="D42" s="2">
+        <v>33</v>
+      </c>
       <c r="E42" s="2">
         <v>29</v>
       </c>
@@ -2899,10 +3203,16 @@
       <c r="G42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="40"/>
+      <c r="H42" s="11">
+        <v>36</v>
+      </c>
+      <c r="I42" s="12">
+        <v>44461</v>
+      </c>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="41"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -2914,6 +3224,15 @@
       <c r="A43" s="2">
         <v>37</v>
       </c>
+      <c r="B43" s="2">
+        <v>36</v>
+      </c>
+      <c r="C43" s="2">
+        <v>37</v>
+      </c>
+      <c r="D43" s="2">
+        <v>34</v>
+      </c>
       <c r="E43" s="2">
         <v>30</v>
       </c>
@@ -2923,10 +3242,16 @@
       <c r="G43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="40"/>
+      <c r="H43" s="11">
+        <v>37</v>
+      </c>
+      <c r="I43" s="12">
+        <v>44462</v>
+      </c>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -2937,16 +3262,34 @@
       <c r="A44" s="2">
         <v>38</v>
       </c>
+      <c r="B44" s="2">
+        <v>37</v>
+      </c>
+      <c r="C44" s="2">
+        <v>38</v>
+      </c>
+      <c r="D44" s="2">
+        <v>35</v>
+      </c>
+      <c r="E44" s="2">
+        <v>31</v>
+      </c>
       <c r="F44" s="2">
         <v>24</v>
       </c>
       <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="40"/>
+      <c r="H44" s="11">
+        <v>38</v>
+      </c>
+      <c r="I44" s="12">
+        <v>44463</v>
+      </c>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -2958,16 +3301,34 @@
       <c r="A45" s="2">
         <v>39</v>
       </c>
+      <c r="B45" s="2">
+        <v>38</v>
+      </c>
+      <c r="C45" s="2">
+        <v>39</v>
+      </c>
+      <c r="D45" s="2">
+        <v>36</v>
+      </c>
+      <c r="E45" s="2">
+        <v>32</v>
+      </c>
       <c r="F45" s="2">
         <v>25</v>
       </c>
       <c r="G45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="40"/>
+      <c r="H45" s="11">
+        <v>39</v>
+      </c>
+      <c r="I45" s="12">
+        <v>44464</v>
+      </c>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="41"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -2979,16 +3340,34 @@
       <c r="A46" s="2">
         <v>40</v>
       </c>
+      <c r="B46" s="2">
+        <v>39</v>
+      </c>
+      <c r="C46" s="2">
+        <v>40</v>
+      </c>
+      <c r="D46" s="2">
+        <v>37</v>
+      </c>
+      <c r="E46" s="2">
+        <v>33</v>
+      </c>
       <c r="F46" s="2">
         <v>26</v>
       </c>
       <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="40"/>
+      <c r="H46" s="11">
+        <v>40</v>
+      </c>
+      <c r="I46" s="12">
+        <v>44465</v>
+      </c>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="41"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -2999,16 +3378,34 @@
       <c r="A47" s="2">
         <v>41</v>
       </c>
+      <c r="B47" s="2">
+        <v>40</v>
+      </c>
+      <c r="C47" s="2">
+        <v>41</v>
+      </c>
+      <c r="D47" s="2">
+        <v>38</v>
+      </c>
+      <c r="E47" s="2">
+        <v>34</v>
+      </c>
       <c r="F47" s="2">
         <v>27</v>
       </c>
       <c r="G47" s="2">
         <v>11</v>
       </c>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="40"/>
+      <c r="H47" s="11">
+        <v>41</v>
+      </c>
+      <c r="I47" s="12">
+        <v>44466</v>
+      </c>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="41"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -3019,16 +3416,34 @@
       <c r="A48" s="2">
         <v>42</v>
       </c>
+      <c r="B48" s="2">
+        <v>41</v>
+      </c>
+      <c r="C48" s="2">
+        <v>42</v>
+      </c>
+      <c r="D48" s="2">
+        <v>39</v>
+      </c>
+      <c r="E48" s="2">
+        <v>35</v>
+      </c>
       <c r="F48" s="2">
         <v>28</v>
       </c>
       <c r="G48" s="2">
         <v>12</v>
       </c>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="40"/>
+      <c r="H48" s="11">
+        <v>42</v>
+      </c>
+      <c r="I48" s="12">
+        <v>44467</v>
+      </c>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="41"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -3039,16 +3454,34 @@
       <c r="A49" s="2">
         <v>43</v>
       </c>
+      <c r="B49" s="2">
+        <v>42</v>
+      </c>
+      <c r="C49" s="2">
+        <v>43</v>
+      </c>
+      <c r="D49" s="2">
+        <v>40</v>
+      </c>
+      <c r="E49" s="2">
+        <v>36</v>
+      </c>
       <c r="F49" s="2">
         <v>29</v>
       </c>
       <c r="G49" s="2">
         <v>13</v>
       </c>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="40"/>
+      <c r="H49" s="11">
+        <v>43</v>
+      </c>
+      <c r="I49" s="12">
+        <v>44468</v>
+      </c>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="41"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -3058,7 +3491,19 @@
     </row>
     <row r="50" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
+        <v>44</v>
+      </c>
+      <c r="B50" s="2">
         <v>43</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44</v>
+      </c>
+      <c r="D50" s="2">
+        <v>41</v>
+      </c>
+      <c r="E50" s="2">
+        <v>37</v>
       </c>
       <c r="F50" s="2">
         <v>30</v>
@@ -3066,10 +3511,16 @@
       <c r="G50" s="2">
         <v>14</v>
       </c>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="40"/>
+      <c r="H50" s="11">
+        <v>44</v>
+      </c>
+      <c r="I50" s="12">
+        <v>44469</v>
+      </c>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="41"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -3079,15 +3530,36 @@
     </row>
     <row r="51" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B51" s="2">
+        <v>44</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45</v>
+      </c>
+      <c r="D51" s="2">
+        <v>42</v>
+      </c>
+      <c r="E51" s="2">
+        <v>38</v>
+      </c>
+      <c r="F51" s="2">
+        <v>31</v>
       </c>
       <c r="G51" s="2">
         <v>15</v>
       </c>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="40"/>
+      <c r="H51" s="11">
+        <v>45</v>
+      </c>
+      <c r="I51" s="12">
+        <v>44470</v>
+      </c>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="41"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -3097,15 +3569,36 @@
     </row>
     <row r="52" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
+        <v>46</v>
+      </c>
+      <c r="B52" s="2">
+        <v>45</v>
+      </c>
+      <c r="C52" s="2">
+        <v>46</v>
+      </c>
+      <c r="D52" s="2">
         <v>43</v>
+      </c>
+      <c r="E52" s="2">
+        <v>39</v>
+      </c>
+      <c r="F52" s="2">
+        <v>32</v>
       </c>
       <c r="G52" s="2">
         <v>16</v>
       </c>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="40"/>
+      <c r="H52" s="11">
+        <v>46</v>
+      </c>
+      <c r="I52" s="12">
+        <v>44471</v>
+      </c>
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="41"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -3115,15 +3608,33 @@
     </row>
     <row r="53" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="B53" s="2">
+        <v>46</v>
+      </c>
+      <c r="D53" s="2">
+        <v>44</v>
+      </c>
+      <c r="E53" s="2">
+        <v>40</v>
+      </c>
+      <c r="F53" s="2">
+        <v>33</v>
       </c>
       <c r="G53" s="2">
         <v>17</v>
       </c>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="40"/>
+      <c r="H53" s="11">
+        <v>47</v>
+      </c>
+      <c r="I53" s="12">
+        <v>44472</v>
+      </c>
+      <c r="J53" s="40"/>
+      <c r="K53" s="40"/>
+      <c r="L53" s="40"/>
+      <c r="M53" s="41"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -3133,33 +3644,63 @@
     </row>
     <row r="54" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="D54" s="2">
+        <v>45</v>
+      </c>
+      <c r="E54" s="2">
+        <v>41</v>
+      </c>
+      <c r="F54" s="2">
+        <v>34</v>
       </c>
       <c r="G54" s="2">
         <v>18</v>
       </c>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="40"/>
+      <c r="H54" s="11">
+        <v>48</v>
+      </c>
+      <c r="I54" s="12">
+        <v>44473</v>
+      </c>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="41"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
-      <c r="V54" s="33"/>
+      <c r="V54" s="32"/>
       <c r="W54" s="12"/>
       <c r="AT54" s="12"/>
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
-        <v>43</v>
+        <v>49</v>
+      </c>
+      <c r="D55" s="2">
+        <v>46</v>
+      </c>
+      <c r="E55" s="2">
+        <v>42</v>
+      </c>
+      <c r="F55" s="2">
+        <v>35</v>
       </c>
       <c r="G55" s="2">
         <v>19</v>
       </c>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="40"/>
+      <c r="H55" s="11">
+        <v>49</v>
+      </c>
+      <c r="I55" s="12">
+        <v>44474</v>
+      </c>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="41"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -3169,15 +3710,27 @@
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
+        <v>50</v>
+      </c>
+      <c r="E56" s="2">
         <v>43</v>
+      </c>
+      <c r="F56" s="2">
+        <v>36</v>
       </c>
       <c r="G56" s="2">
         <v>20</v>
       </c>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="40"/>
+      <c r="H56" s="11">
+        <v>50</v>
+      </c>
+      <c r="I56" s="12">
+        <v>44475</v>
+      </c>
+      <c r="J56" s="40"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="41"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -3187,15 +3740,27 @@
     </row>
     <row r="57" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
-        <v>43</v>
+        <v>51</v>
+      </c>
+      <c r="E57" s="2">
+        <v>44</v>
+      </c>
+      <c r="F57" s="2">
+        <v>37</v>
       </c>
       <c r="G57" s="2">
         <v>21</v>
       </c>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="40"/>
+      <c r="H57" s="11">
+        <v>51</v>
+      </c>
+      <c r="I57" s="12">
+        <v>44476</v>
+      </c>
+      <c r="J57" s="40"/>
+      <c r="K57" s="40"/>
+      <c r="L57" s="40"/>
+      <c r="M57" s="41"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -3205,15 +3770,27 @@
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="E58" s="2">
+        <v>45</v>
+      </c>
+      <c r="F58" s="2">
+        <v>38</v>
       </c>
       <c r="G58" s="2">
         <v>22</v>
       </c>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="40"/>
+      <c r="H58" s="11">
+        <v>52</v>
+      </c>
+      <c r="I58" s="12">
+        <v>44477</v>
+      </c>
+      <c r="J58" s="40"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="41"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -3223,15 +3800,27 @@
     </row>
     <row r="59" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="E59" s="2">
+        <v>46</v>
+      </c>
+      <c r="F59" s="2">
+        <v>39</v>
       </c>
       <c r="G59" s="2">
         <v>23</v>
       </c>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="40"/>
+      <c r="H59" s="11">
+        <v>53</v>
+      </c>
+      <c r="I59" s="12">
+        <v>44478</v>
+      </c>
+      <c r="J59" s="40"/>
+      <c r="K59" s="40"/>
+      <c r="L59" s="40"/>
+      <c r="M59" s="41"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -3241,15 +3830,24 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="F60" s="2">
+        <v>40</v>
       </c>
       <c r="G60" s="2">
         <v>24</v>
       </c>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="40"/>
+      <c r="H60" s="11">
+        <v>54</v>
+      </c>
+      <c r="I60" s="12">
+        <v>44479</v>
+      </c>
+      <c r="J60" s="40"/>
+      <c r="K60" s="40"/>
+      <c r="L60" s="40"/>
+      <c r="M60" s="41"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -3257,15 +3855,24 @@
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="F61" s="2">
+        <v>41</v>
       </c>
       <c r="G61" s="2">
         <v>25</v>
       </c>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="40"/>
+      <c r="H61" s="11">
+        <v>55</v>
+      </c>
+      <c r="I61" s="12">
+        <v>44480</v>
+      </c>
+      <c r="J61" s="40"/>
+      <c r="K61" s="40"/>
+      <c r="L61" s="40"/>
+      <c r="M61" s="41"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -3276,15 +3883,24 @@
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
-        <v>43</v>
+        <v>56</v>
+      </c>
+      <c r="F62" s="2">
+        <v>42</v>
       </c>
       <c r="G62" s="2">
         <v>26</v>
       </c>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="40"/>
+      <c r="H62" s="11">
+        <v>56</v>
+      </c>
+      <c r="I62" s="12">
+        <v>44481</v>
+      </c>
+      <c r="J62" s="40"/>
+      <c r="K62" s="40"/>
+      <c r="L62" s="40"/>
+      <c r="M62" s="41"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -3294,15 +3910,24 @@
     </row>
     <row r="63" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
+        <v>57</v>
+      </c>
+      <c r="F63" s="2">
         <v>43</v>
       </c>
       <c r="G63" s="2">
         <v>27</v>
       </c>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
-      <c r="M63" s="40"/>
+      <c r="H63" s="11">
+        <v>57</v>
+      </c>
+      <c r="I63" s="12">
+        <v>44482</v>
+      </c>
+      <c r="J63" s="40"/>
+      <c r="K63" s="40"/>
+      <c r="L63" s="40"/>
+      <c r="M63" s="41"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -3312,15 +3937,24 @@
     </row>
     <row r="64" spans="1:46" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
-        <v>43</v>
+        <v>58</v>
+      </c>
+      <c r="F64" s="2">
+        <v>44</v>
       </c>
       <c r="G64" s="2">
         <v>28</v>
       </c>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="40"/>
+      <c r="H64" s="11">
+        <v>58</v>
+      </c>
+      <c r="I64" s="12">
+        <v>44483</v>
+      </c>
+      <c r="J64" s="40"/>
+      <c r="K64" s="40"/>
+      <c r="L64" s="40"/>
+      <c r="M64" s="41"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -3329,99 +3963,312 @@
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
-        <v>43</v>
+        <v>59</v>
+      </c>
+      <c r="F65" s="2">
+        <v>45</v>
       </c>
       <c r="G65" s="2">
         <v>29</v>
       </c>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="40"/>
+      <c r="H65" s="11">
+        <v>59</v>
+      </c>
+      <c r="I65" s="12">
+        <v>44484</v>
+      </c>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40"/>
+      <c r="L65" s="40"/>
+      <c r="M65" s="41"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A66" s="2">
+        <v>60</v>
+      </c>
+      <c r="F66" s="2">
+        <v>46</v>
+      </c>
       <c r="G66" s="2">
         <v>30</v>
       </c>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="40"/>
+      <c r="H66" s="11">
+        <v>60</v>
+      </c>
+      <c r="I66" s="12">
+        <v>44485</v>
+      </c>
+      <c r="J66" s="40"/>
+      <c r="K66" s="40"/>
+      <c r="L66" s="40"/>
+      <c r="M66" s="41"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A67" s="2">
+        <v>61</v>
+      </c>
+      <c r="G67" s="2">
+        <v>31</v>
+      </c>
+      <c r="H67" s="11">
+        <v>61</v>
+      </c>
+      <c r="I67" s="12">
+        <v>44486</v>
+      </c>
       <c r="S67" s="12"/>
       <c r="T67" s="12"/>
       <c r="U67" s="12"/>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A68" s="2">
+        <v>62</v>
+      </c>
+      <c r="G68" s="2">
+        <v>32</v>
+      </c>
+      <c r="H68" s="11">
+        <v>62</v>
+      </c>
+      <c r="I68" s="12">
+        <v>44487</v>
+      </c>
       <c r="U68" s="12"/>
-      <c r="V68" s="33"/>
+      <c r="V68" s="32"/>
       <c r="W68" s="12"/>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A69" s="2">
+        <v>63</v>
+      </c>
+      <c r="G69" s="2">
+        <v>33</v>
+      </c>
+      <c r="H69" s="11">
+        <v>63</v>
+      </c>
+      <c r="I69" s="12">
+        <v>44488</v>
+      </c>
       <c r="W69" s="12"/>
       <c r="X69" s="12"/>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A70" s="2">
+        <v>64</v>
+      </c>
+      <c r="G70" s="2">
+        <v>34</v>
+      </c>
+      <c r="H70" s="11">
+        <v>64</v>
+      </c>
+      <c r="I70" s="12">
+        <v>44489</v>
+      </c>
       <c r="Y70" s="12"/>
       <c r="Z70" s="12"/>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A71" s="2">
+        <v>65</v>
+      </c>
+      <c r="G71" s="2">
+        <v>35</v>
+      </c>
+      <c r="H71" s="11">
+        <v>65</v>
+      </c>
+      <c r="I71" s="12">
+        <v>44490</v>
+      </c>
       <c r="AA71" s="12"/>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A72" s="2">
+        <v>66</v>
+      </c>
+      <c r="G72" s="2">
+        <v>36</v>
+      </c>
+      <c r="H72" s="11">
+        <v>66</v>
+      </c>
+      <c r="I72" s="12">
+        <v>44491</v>
+      </c>
       <c r="AB72" s="12"/>
       <c r="AC72" s="12"/>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A73" s="2">
+        <v>67</v>
+      </c>
+      <c r="G73" s="2">
+        <v>37</v>
+      </c>
+      <c r="H73" s="11">
+        <v>67</v>
+      </c>
+      <c r="I73" s="12">
+        <v>44492</v>
+      </c>
       <c r="AD73" s="12"/>
       <c r="AE73" s="12"/>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A74" s="2">
+        <v>68</v>
+      </c>
+      <c r="G74" s="2">
+        <v>38</v>
+      </c>
+      <c r="H74" s="11">
+        <v>68</v>
+      </c>
+      <c r="I74" s="12">
+        <v>44493</v>
+      </c>
       <c r="AF74" s="12"/>
       <c r="AG74" s="12"/>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A75" s="2">
+        <v>69</v>
+      </c>
+      <c r="G75" s="2">
+        <v>39</v>
+      </c>
+      <c r="H75" s="11">
+        <v>69</v>
+      </c>
+      <c r="I75" s="12">
+        <v>44494</v>
+      </c>
       <c r="AH75" s="12"/>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A76" s="2">
+        <v>70</v>
+      </c>
+      <c r="G76" s="2">
+        <v>40</v>
+      </c>
+      <c r="H76" s="11">
+        <v>70</v>
+      </c>
+      <c r="I76" s="12">
+        <v>44495</v>
+      </c>
       <c r="AI76" s="12"/>
       <c r="AJ76" s="12"/>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A77" s="2">
+        <v>71</v>
+      </c>
+      <c r="G77" s="2">
+        <v>41</v>
+      </c>
+      <c r="H77" s="11">
+        <v>71</v>
+      </c>
+      <c r="I77" s="12">
+        <v>44496</v>
+      </c>
       <c r="AK77" s="12"/>
       <c r="AL77" s="12"/>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A78" s="2">
+        <v>72</v>
+      </c>
+      <c r="G78" s="2">
+        <v>42</v>
+      </c>
+      <c r="H78" s="11">
+        <v>72</v>
+      </c>
+      <c r="I78" s="12">
+        <v>44497</v>
+      </c>
       <c r="AM78" s="12"/>
       <c r="AN78" s="12"/>
       <c r="AO78" s="12"/>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A79" s="2">
+        <v>73</v>
+      </c>
+      <c r="G79" s="2">
+        <v>43</v>
+      </c>
+      <c r="H79" s="11">
+        <v>73</v>
+      </c>
+      <c r="I79" s="12">
+        <v>44498</v>
+      </c>
       <c r="AP79" s="12"/>
       <c r="AQ79" s="12"/>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.45">
+      <c r="A80" s="2">
+        <v>74</v>
+      </c>
+      <c r="G80" s="2">
+        <v>44</v>
+      </c>
+      <c r="H80" s="11">
+        <v>74</v>
+      </c>
+      <c r="I80" s="12">
+        <v>44499</v>
+      </c>
       <c r="AR80" s="12"/>
     </row>
-    <row r="81" spans="13:46" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="A81" s="2">
+        <v>75</v>
+      </c>
+      <c r="G81" s="2">
+        <v>45</v>
+      </c>
+      <c r="H81" s="11">
+        <v>75</v>
+      </c>
+      <c r="I81" s="12">
+        <v>44500</v>
+      </c>
       <c r="AS81" s="12"/>
       <c r="AT81" s="12"/>
     </row>
-    <row r="82" spans="13:46" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.45">
+      <c r="A82" s="2">
+        <v>76</v>
+      </c>
+      <c r="G82" s="2">
+        <v>46</v>
+      </c>
+      <c r="H82" s="11">
+        <v>76</v>
+      </c>
+      <c r="I82" s="12">
+        <v>44501</v>
+      </c>
       <c r="M82" s="13"/>
       <c r="N82" s="12"/>
     </row>
-    <row r="83" spans="13:46" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.45">
       <c r="O83" s="12"/>
     </row>
-    <row r="84" spans="13:46" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.45">
       <c r="P84" s="12"/>
       <c r="Q84" s="12"/>
     </row>

</xml_diff>

<commit_message>
:tada:[ADD] 복습 - 18일차
오래된 부분에서 했던 실수를 반복하는 경향이 있음. 자료형을 제대로 확인하고 입력받자.

기존에 잘못 알고 있던 부분들도 많이 보였음. 이렇게 하면 반드시 틀리는데, 그냥 넘어간 이유는 테스트케이스가 부족해서 맞은줄 알고 넘어갔던 것. (즉, 코드를 제대로 이해하지 못했던 것.)

실수를 다시 잡자. 그리고 다시는 하지 말자.
</commit_message>
<xml_diff>
--- a/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
+++ b/이것이 코딩 테스트다 with 파이썬/코딩테스트 복습주기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\이것이 코딩 테스트다 with 파이썬\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB394B-3984-44D3-BE44-7330EA61457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A0FF6D-88E9-4E17-BF8F-BABE5D5D0F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="640" windowWidth="23200" windowHeight="20360" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
+    <workbookView xWindow="2920" yWindow="610" windowWidth="23200" windowHeight="20360" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -901,119 +901,119 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:AT84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1365,116 +1365,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77" t="s">
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76" t="s">
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76" t="s">
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="64" t="s">
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
     </row>
     <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:36" s="6" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
       <c r="H3" s="38" t="s">
         <v>29</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="51"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="61"/>
       <c r="V3" s="29"/>
     </row>
     <row r="4" spans="1:36" s="8" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -1487,17 +1487,17 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="54"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="64"/>
       <c r="V4" s="30"/>
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
@@ -1520,15 +1520,15 @@
       <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="61" t="s">
+      <c r="H5" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="62"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="55" t="s">
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="56"/>
+      <c r="L5" s="66"/>
       <c r="M5" s="24" t="s">
         <v>32</v>
       </c>
@@ -1564,14 +1564,14 @@
       <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="59"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="69"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1610,12 +1610,12 @@
       <c r="I7" s="12">
         <v>44417</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="43"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -1663,12 +1663,12 @@
       <c r="I8" s="12">
         <v>44418</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="43"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="55"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -1701,12 +1701,12 @@
       <c r="I9" s="12">
         <v>44419</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="45"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="72"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -1758,12 +1758,12 @@
       <c r="I10" s="12">
         <v>44423</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="43"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="55"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -1802,12 +1802,12 @@
       <c r="I11" s="12">
         <v>44424</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="43"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -1906,12 +1906,12 @@
       <c r="I13" s="12">
         <v>44426</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="43"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -1995,7 +1995,7 @@
       <c r="Y14" s="37"/>
       <c r="Z14" s="37"/>
       <c r="AA14" s="37"/>
-      <c r="AB14" s="15"/>
+      <c r="AB14" s="37"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
@@ -2019,12 +2019,12 @@
       <c r="I15" s="12">
         <v>44429</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="43"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="55"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -2084,12 +2084,12 @@
       <c r="I16" s="12">
         <v>44431</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="72"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -2134,12 +2134,12 @@
       <c r="I17" s="12">
         <v>44433</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="43"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -2199,12 +2199,12 @@
       <c r="I18" s="12">
         <v>44434</v>
       </c>
-      <c r="J18" s="42" t="s">
+      <c r="J18" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="43"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="55"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -2251,12 +2251,12 @@
       <c r="I19" s="12">
         <v>44438</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -2316,12 +2316,12 @@
       <c r="I20" s="12">
         <v>44439</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="43"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="55"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -2369,12 +2369,12 @@
       <c r="I21" s="12">
         <v>44440</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="45"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="72"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -2441,12 +2441,12 @@
       <c r="I22" s="12">
         <v>44441</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="45"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="72"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -2497,12 +2497,12 @@
       <c r="I23" s="12">
         <v>44442</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="43"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -2535,19 +2535,19 @@
       <c r="A24" s="2">
         <v>18</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="10">
         <v>17</v>
       </c>
       <c r="C24" s="2">
         <v>18</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="10">
         <v>15</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="10">
         <v>11</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="10">
         <v>4</v>
       </c>
       <c r="H24" s="11">
@@ -2556,12 +2556,25 @@
       <c r="I24" s="12">
         <v>44443</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="41"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="77"/>
       <c r="N24" s="2">
         <v>18</v>
+      </c>
+      <c r="O24" s="12">
+        <v>44443</v>
+      </c>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12">
+        <v>44443</v>
+      </c>
+      <c r="R24" s="12">
+        <v>44443</v>
+      </c>
+      <c r="S24" s="12">
+        <v>44443</v>
       </c>
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
@@ -2591,10 +2604,10 @@
       <c r="I25" s="12">
         <v>44444</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="41"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="77"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -2625,10 +2638,10 @@
       <c r="I26" s="12">
         <v>44445</v>
       </c>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="41"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="77"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -2660,10 +2673,10 @@
       <c r="I27" s="12">
         <v>44446</v>
       </c>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="41"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="77"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -2695,10 +2708,10 @@
       <c r="I28" s="12">
         <v>44447</v>
       </c>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="41"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="77"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -2729,10 +2742,10 @@
       <c r="I29" s="12">
         <v>44448</v>
       </c>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="41"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="77"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -2765,10 +2778,10 @@
       <c r="I30" s="12">
         <v>44449</v>
       </c>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="41"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="77"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -2801,10 +2814,10 @@
       <c r="I31" s="12">
         <v>44450</v>
       </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="41"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="76"/>
+      <c r="M31" s="77"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -2837,10 +2850,10 @@
       <c r="I32" s="12">
         <v>44451</v>
       </c>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="41"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="76"/>
+      <c r="L32" s="76"/>
+      <c r="M32" s="77"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -2873,10 +2886,10 @@
       <c r="I33" s="12">
         <v>44452</v>
       </c>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="41"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="76"/>
+      <c r="L33" s="76"/>
+      <c r="M33" s="77"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -2909,10 +2922,10 @@
       <c r="I34" s="12">
         <v>44453</v>
       </c>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="41"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="77"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -2945,10 +2958,10 @@
       <c r="I35" s="12">
         <v>44454</v>
       </c>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="41"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="77"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -2981,10 +2994,10 @@
       <c r="I36" s="12">
         <v>44455</v>
       </c>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="41"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="77"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -3020,10 +3033,10 @@
       <c r="I37" s="12">
         <v>44456</v>
       </c>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="41"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="77"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -3058,10 +3071,10 @@
       <c r="I38" s="12">
         <v>44457</v>
       </c>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="41"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="77"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -3095,10 +3108,10 @@
       <c r="I39" s="12">
         <v>44458</v>
       </c>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="41"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="77"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -3132,10 +3145,10 @@
       <c r="I40" s="12">
         <v>44459</v>
       </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="41"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="77"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
@@ -3170,10 +3183,10 @@
       <c r="I41" s="12">
         <v>44460</v>
       </c>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="41"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="77"/>
       <c r="N41" s="2">
         <v>35</v>
       </c>
@@ -3209,10 +3222,10 @@
       <c r="I42" s="12">
         <v>44461</v>
       </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="41"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="77"/>
       <c r="N42" s="2">
         <v>36</v>
       </c>
@@ -3248,10 +3261,10 @@
       <c r="I43" s="12">
         <v>44462</v>
       </c>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="41"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="77"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
@@ -3286,10 +3299,10 @@
       <c r="I44" s="12">
         <v>44463</v>
       </c>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="41"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="77"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -3325,10 +3338,10 @@
       <c r="I45" s="12">
         <v>44464</v>
       </c>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="41"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="77"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -3364,10 +3377,10 @@
       <c r="I46" s="12">
         <v>44465</v>
       </c>
-      <c r="J46" s="40"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="41"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="76"/>
+      <c r="L46" s="76"/>
+      <c r="M46" s="77"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
@@ -3402,10 +3415,10 @@
       <c r="I47" s="12">
         <v>44466</v>
       </c>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="41"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="77"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
@@ -3440,10 +3453,10 @@
       <c r="I48" s="12">
         <v>44467</v>
       </c>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="41"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="77"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
@@ -3478,10 +3491,10 @@
       <c r="I49" s="12">
         <v>44468</v>
       </c>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="41"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="77"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -3517,10 +3530,10 @@
       <c r="I50" s="12">
         <v>44469</v>
       </c>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="41"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="77"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -3556,10 +3569,10 @@
       <c r="I51" s="12">
         <v>44470</v>
       </c>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="41"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="77"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -3595,10 +3608,10 @@
       <c r="I52" s="12">
         <v>44471</v>
       </c>
-      <c r="J52" s="40"/>
-      <c r="K52" s="40"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="41"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="77"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -3631,10 +3644,10 @@
       <c r="I53" s="12">
         <v>44472</v>
       </c>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="41"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="77"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -3664,10 +3677,10 @@
       <c r="I54" s="12">
         <v>44473</v>
       </c>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="41"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
+      <c r="M54" s="77"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -3697,10 +3710,10 @@
       <c r="I55" s="12">
         <v>44474</v>
       </c>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="40"/>
-      <c r="M55" s="41"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="77"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -3727,10 +3740,10 @@
       <c r="I56" s="12">
         <v>44475</v>
       </c>
-      <c r="J56" s="40"/>
-      <c r="K56" s="40"/>
-      <c r="L56" s="40"/>
-      <c r="M56" s="41"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="77"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -3757,10 +3770,10 @@
       <c r="I57" s="12">
         <v>44476</v>
       </c>
-      <c r="J57" s="40"/>
-      <c r="K57" s="40"/>
-      <c r="L57" s="40"/>
-      <c r="M57" s="41"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="77"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -3787,10 +3800,10 @@
       <c r="I58" s="12">
         <v>44477</v>
       </c>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
-      <c r="L58" s="40"/>
-      <c r="M58" s="41"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="76"/>
+      <c r="M58" s="77"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -3817,10 +3830,10 @@
       <c r="I59" s="12">
         <v>44478</v>
       </c>
-      <c r="J59" s="40"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="40"/>
-      <c r="M59" s="41"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="76"/>
+      <c r="M59" s="77"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -3844,10 +3857,10 @@
       <c r="I60" s="12">
         <v>44479</v>
       </c>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="41"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="77"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
@@ -3869,10 +3882,10 @@
       <c r="I61" s="12">
         <v>44480</v>
       </c>
-      <c r="J61" s="40"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="40"/>
-      <c r="M61" s="41"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="76"/>
+      <c r="M61" s="77"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -3897,10 +3910,10 @@
       <c r="I62" s="12">
         <v>44481</v>
       </c>
-      <c r="J62" s="40"/>
-      <c r="K62" s="40"/>
-      <c r="L62" s="40"/>
-      <c r="M62" s="41"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="76"/>
+      <c r="M62" s="77"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -3924,10 +3937,10 @@
       <c r="I63" s="12">
         <v>44482</v>
       </c>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
-      <c r="L63" s="40"/>
-      <c r="M63" s="41"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="76"/>
+      <c r="M63" s="77"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -3951,10 +3964,10 @@
       <c r="I64" s="12">
         <v>44483</v>
       </c>
-      <c r="J64" s="40"/>
-      <c r="K64" s="40"/>
-      <c r="L64" s="40"/>
-      <c r="M64" s="41"/>
+      <c r="J64" s="76"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="76"/>
+      <c r="M64" s="77"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
@@ -3977,10 +3990,10 @@
       <c r="I65" s="12">
         <v>44484</v>
       </c>
-      <c r="J65" s="40"/>
-      <c r="K65" s="40"/>
-      <c r="L65" s="40"/>
-      <c r="M65" s="41"/>
+      <c r="J65" s="76"/>
+      <c r="K65" s="76"/>
+      <c r="L65" s="76"/>
+      <c r="M65" s="77"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
@@ -4001,10 +4014,10 @@
       <c r="I66" s="12">
         <v>44485</v>
       </c>
-      <c r="J66" s="40"/>
-      <c r="K66" s="40"/>
-      <c r="L66" s="40"/>
-      <c r="M66" s="41"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="76"/>
+      <c r="M66" s="77"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
@@ -4274,18 +4287,59 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
@@ -4300,59 +4354,18 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>